<commit_message>
UML et fichier fin projet
Fin des uml et création et début de remplissage du fichier pour la fin du projet (donée déjà disponibles)
</commit_message>
<xml_diff>
--- a/documents/AutoEval_Dussault_Morgan.xlsx
+++ b/documents/AutoEval_Dussault_Morgan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px05iql\OneDrive - Education Vaud\Cours\2022-2023\T1\P_DEV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg66hua\Documents\GitHub\Space-invader\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_029BF6AA61B32D47C019AED4CCE34CF8E73B1BDF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77E2315-8F5C-4BE8-B69F-4B71B46FE6EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dussault_Morgan" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,25 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Dussault_Morgan!$A$1:$S$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
   <si>
     <t xml:space="preserve">ÉVALUATION DES COMPÉTENCES EN PRATIQUE POUR LA FORMATION </t>
   </si>
@@ -79,6 +87,9 @@
   <si>
     <t xml:space="preserve">Enseignant : </t>
   </si>
+  <si>
+    <t>Dussault Morgan</t>
+  </si>
 </sst>
 </file>
 
@@ -1571,6 +1582,83 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="37" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1598,83 +1686,6 @@
     <xf numFmtId="164" fontId="43" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="38" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -2318,11 +2329,11 @@
   </sheetPr>
   <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="13.15" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="13.15" customHeight="1" zeroHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="6" customWidth="1"/>
@@ -2361,11 +2372,11 @@
       <c r="M1" s="4"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="195" t="s">
+      <c r="P1" s="172" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="195"/>
-      <c r="R1" s="195"/>
+      <c r="Q1" s="172"/>
+      <c r="R1" s="172"/>
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:23" ht="37.5" customHeight="1">
@@ -2453,14 +2464,14 @@
       <c r="M4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="196" t="str">
+      <c r="N4" s="173" t="str">
         <f>[1]Automation!F12</f>
         <v>29.8.2022 - 9.1.2023</v>
       </c>
-      <c r="O4" s="196"/>
-      <c r="P4" s="196"/>
-      <c r="Q4" s="196"/>
-      <c r="R4" s="196"/>
+      <c r="O4" s="173"/>
+      <c r="P4" s="173"/>
+      <c r="Q4" s="173"/>
+      <c r="R4" s="173"/>
       <c r="S4" s="27"/>
     </row>
     <row r="5" spans="1:23" s="28" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -2500,34 +2511,34 @@
     <row r="7" spans="1:23" s="50" customFormat="1" ht="70.150000000000006" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="49"/>
       <c r="D7" s="51"/>
-      <c r="E7" s="197" t="str">
+      <c r="E7" s="174" t="str">
         <f>[1]INDICATEURS!E7</f>
         <v>LARGEMENT ACQUIS
 5.5 ou 6.0</v>
       </c>
-      <c r="F7" s="198"/>
-      <c r="G7" s="198"/>
-      <c r="H7" s="199" t="str">
+      <c r="F7" s="175"/>
+      <c r="G7" s="175"/>
+      <c r="H7" s="176" t="str">
         <f>[1]INDICATEURS!H7</f>
         <v>SUFFISANT
 4.0, 4.5 ou 5.0</v>
       </c>
-      <c r="I7" s="200"/>
-      <c r="J7" s="200"/>
-      <c r="K7" s="201" t="str">
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="178" t="str">
         <f>[1]INDICATEURS!K7</f>
         <v>INSUFFISANT
 2.5, 3.0 ou 3.5</v>
       </c>
-      <c r="L7" s="202"/>
-      <c r="M7" s="202"/>
-      <c r="N7" s="203" t="str">
+      <c r="L7" s="179"/>
+      <c r="M7" s="179"/>
+      <c r="N7" s="180" t="str">
         <f>[1]INDICATEURS!N7</f>
         <v>NON ACQUIS
 1.0, 1.5, ou 2.0</v>
       </c>
-      <c r="O7" s="204"/>
-      <c r="P7" s="204"/>
+      <c r="O7" s="181"/>
+      <c r="P7" s="181"/>
       <c r="Q7" s="52" t="str">
         <f>[1]INDICATEURS!Q7</f>
         <v>Coeff.</v>
@@ -2541,11 +2552,11 @@
     </row>
     <row r="8" spans="1:23" ht="100.15" customHeight="1" thickTop="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="184" t="str">
+      <c r="B8" s="182" t="str">
         <f>[1]INDICATEURS!B8</f>
         <v>COMPÉTENCES</v>
       </c>
-      <c r="C8" s="187" t="str">
+      <c r="C8" s="185" t="str">
         <f>[1]INDICATEURS!C8</f>
         <v>PROFESSIONNELLES</v>
       </c>
@@ -2599,8 +2610,8 @@
     </row>
     <row r="9" spans="1:23" ht="100.15" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="185"/>
-      <c r="C9" s="188"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="186"/>
       <c r="D9" s="71" t="str">
         <f>[1]INDICATEURS!D9</f>
         <v>Conscience professionnelle
@@ -2651,8 +2662,8 @@
     </row>
     <row r="10" spans="1:23" ht="100.15" customHeight="1" thickBot="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="185"/>
-      <c r="C10" s="188"/>
+      <c r="B10" s="183"/>
+      <c r="C10" s="186"/>
       <c r="D10" s="71" t="str">
         <f>[1]INDICATEURS!D10</f>
         <v>Connaissances professionnelles
@@ -2703,8 +2714,8 @@
     </row>
     <row r="11" spans="1:23" ht="100.15" customHeight="1" thickTop="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="185"/>
-      <c r="C11" s="189" t="str">
+      <c r="B11" s="183"/>
+      <c r="C11" s="187" t="str">
         <f>[1]INDICATEURS!C11</f>
         <v>METHODOLOGIQUES</v>
       </c>
@@ -2757,8 +2768,8 @@
     </row>
     <row r="12" spans="1:23" ht="100.15" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="185"/>
-      <c r="C12" s="190"/>
+      <c r="B12" s="183"/>
+      <c r="C12" s="188"/>
       <c r="D12" s="102" t="str">
         <f>[1]INDICATEURS!D12</f>
         <v>Expression orale et écrite
@@ -2809,8 +2820,8 @@
     </row>
     <row r="13" spans="1:23" ht="100.15" customHeight="1" thickBot="1">
       <c r="A13" s="7"/>
-      <c r="B13" s="185"/>
-      <c r="C13" s="191"/>
+      <c r="B13" s="183"/>
+      <c r="C13" s="189"/>
       <c r="D13" s="117" t="str">
         <f>[1]INDICATEURS!D13</f>
         <v>Approche écologique et économique
@@ -2832,7 +2843,7 @@
         <v>Utilise les technologies et moyens qui ménagent les ressources et les coûts</v>
       </c>
       <c r="J13" s="121">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K13" s="90" t="s">
         <v>9</v>
@@ -2861,7 +2872,7 @@
     </row>
     <row r="14" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="7"/>
-      <c r="B14" s="185"/>
+      <c r="B14" s="183"/>
       <c r="C14" s="128" t="str">
         <f>[1]INDICATEURS!C14</f>
         <v>SOCIALES</v>
@@ -2916,7 +2927,7 @@
     </row>
     <row r="15" spans="1:23" ht="120" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="7"/>
-      <c r="B15" s="186"/>
+      <c r="B15" s="184"/>
       <c r="C15" s="128" t="str">
         <f>[1]INDICATEURS!C15</f>
         <v>PERSONNELLES</v>
@@ -2988,7 +2999,7 @@
       <c r="M17" s="151"/>
       <c r="N17" s="153"/>
       <c r="O17" s="154"/>
-      <c r="P17" s="192" t="s">
+      <c r="P17" s="190" t="s">
         <v>11</v>
       </c>
       <c r="Q17" s="155"/>
@@ -3004,43 +3015,43 @@
       <c r="M18" s="152"/>
       <c r="N18" s="152"/>
       <c r="O18" s="152"/>
-      <c r="P18" s="192"/>
+      <c r="P18" s="190"/>
       <c r="Q18" s="155"/>
       <c r="R18" s="155"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="1:19" ht="30" customHeight="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="193"/>
-      <c r="C19" s="193"/>
-      <c r="D19" s="193"/>
-      <c r="E19" s="193"/>
-      <c r="F19" s="193"/>
-      <c r="G19" s="193"/>
-      <c r="H19" s="193"/>
-      <c r="I19" s="193"/>
-      <c r="K19" s="205" t="s">
+      <c r="B19" s="191"/>
+      <c r="C19" s="191"/>
+      <c r="D19" s="191"/>
+      <c r="E19" s="191"/>
+      <c r="F19" s="191"/>
+      <c r="G19" s="191"/>
+      <c r="H19" s="191"/>
+      <c r="I19" s="191"/>
+      <c r="K19" s="192" t="s">
         <v>12</v>
       </c>
-      <c r="L19" s="205"/>
-      <c r="M19" s="194"/>
-      <c r="N19" s="194"/>
-      <c r="O19" s="194"/>
-      <c r="P19" s="192"/>
+      <c r="L19" s="192"/>
+      <c r="M19" s="193"/>
+      <c r="N19" s="193"/>
+      <c r="O19" s="193"/>
+      <c r="P19" s="190"/>
       <c r="Q19" s="155"/>
       <c r="R19" s="155"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="1:19" ht="30" customHeight="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="181"/>
-      <c r="C20" s="181"/>
-      <c r="D20" s="181"/>
-      <c r="E20" s="181"/>
-      <c r="F20" s="181"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="181"/>
+      <c r="B20" s="194"/>
+      <c r="C20" s="194"/>
+      <c r="D20" s="194"/>
+      <c r="E20" s="194"/>
+      <c r="F20" s="194"/>
+      <c r="G20" s="194"/>
+      <c r="H20" s="194"/>
+      <c r="I20" s="194"/>
       <c r="K20" s="158"/>
       <c r="L20" s="158"/>
       <c r="M20" s="152"/>
@@ -3053,21 +3064,23 @@
     </row>
     <row r="21" spans="1:19" ht="30" customHeight="1">
       <c r="A21" s="7"/>
-      <c r="B21" s="181"/>
-      <c r="C21" s="181"/>
-      <c r="D21" s="181"/>
-      <c r="E21" s="181"/>
-      <c r="F21" s="181"/>
-      <c r="G21" s="181"/>
-      <c r="H21" s="181"/>
-      <c r="I21" s="181"/>
-      <c r="K21" s="182" t="s">
+      <c r="B21" s="194"/>
+      <c r="C21" s="194"/>
+      <c r="D21" s="194"/>
+      <c r="E21" s="194"/>
+      <c r="F21" s="194"/>
+      <c r="G21" s="194"/>
+      <c r="H21" s="194"/>
+      <c r="I21" s="194"/>
+      <c r="K21" s="195" t="s">
         <v>13</v>
       </c>
-      <c r="L21" s="182"/>
-      <c r="M21" s="183"/>
-      <c r="N21" s="183"/>
-      <c r="O21" s="183"/>
+      <c r="L21" s="195"/>
+      <c r="M21" s="196" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" s="196"/>
+      <c r="O21" s="196"/>
       <c r="P21" s="161"/>
       <c r="Q21" s="162"/>
       <c r="R21" s="162"/>
@@ -3075,14 +3088,14 @@
     </row>
     <row r="22" spans="1:19" ht="30" customHeight="1">
       <c r="A22" s="7"/>
-      <c r="B22" s="181"/>
-      <c r="C22" s="181"/>
-      <c r="D22" s="181"/>
-      <c r="E22" s="181"/>
-      <c r="F22" s="181"/>
-      <c r="G22" s="181"/>
-      <c r="H22" s="181"/>
-      <c r="I22" s="181"/>
+      <c r="B22" s="194"/>
+      <c r="C22" s="194"/>
+      <c r="D22" s="194"/>
+      <c r="E22" s="194"/>
+      <c r="F22" s="194"/>
+      <c r="G22" s="194"/>
+      <c r="H22" s="194"/>
+      <c r="I22" s="194"/>
       <c r="K22" s="152"/>
       <c r="L22" s="152"/>
       <c r="M22" s="152"/>
@@ -3094,112 +3107,112 @@
     </row>
     <row r="23" spans="1:19" ht="30" customHeight="1">
       <c r="A23" s="7"/>
-      <c r="B23" s="181"/>
-      <c r="C23" s="181"/>
-      <c r="D23" s="181"/>
-      <c r="E23" s="181"/>
-      <c r="F23" s="181"/>
-      <c r="G23" s="181"/>
-      <c r="H23" s="181"/>
-      <c r="I23" s="181"/>
+      <c r="B23" s="194"/>
+      <c r="C23" s="194"/>
+      <c r="D23" s="194"/>
+      <c r="E23" s="194"/>
+      <c r="F23" s="194"/>
+      <c r="G23" s="194"/>
+      <c r="H23" s="194"/>
+      <c r="I23" s="194"/>
       <c r="J23" s="163"/>
       <c r="K23" s="151" t="s">
         <v>14</v>
       </c>
       <c r="L23" s="164"/>
-      <c r="M23" s="183"/>
-      <c r="N23" s="183"/>
-      <c r="O23" s="183"/>
-      <c r="P23" s="173"/>
-      <c r="Q23" s="175" t="str">
+      <c r="M23" s="196"/>
+      <c r="N23" s="196"/>
+      <c r="O23" s="196"/>
+      <c r="P23" s="198"/>
+      <c r="Q23" s="200" t="str">
         <f>IF(COUNT(R8:R15)=8,MROUND(SUM(R8:R15)/SUM(Q8:Q15),0.5),"")</f>
         <v/>
       </c>
-      <c r="R23" s="176"/>
+      <c r="R23" s="201"/>
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:19" ht="30" customHeight="1">
       <c r="A24" s="7"/>
-      <c r="B24" s="181"/>
-      <c r="C24" s="181"/>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="181"/>
+      <c r="B24" s="194"/>
+      <c r="C24" s="194"/>
+      <c r="D24" s="194"/>
+      <c r="E24" s="194"/>
+      <c r="F24" s="194"/>
+      <c r="G24" s="194"/>
+      <c r="H24" s="194"/>
+      <c r="I24" s="194"/>
       <c r="J24" s="165"/>
       <c r="K24" s="152"/>
       <c r="L24" s="151"/>
       <c r="M24" s="151"/>
       <c r="N24" s="151"/>
       <c r="O24" s="166"/>
-      <c r="P24" s="174"/>
-      <c r="Q24" s="177"/>
-      <c r="R24" s="178"/>
+      <c r="P24" s="199"/>
+      <c r="Q24" s="202"/>
+      <c r="R24" s="203"/>
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="1:19" ht="28.5" customHeight="1">
       <c r="A25" s="7"/>
-      <c r="B25" s="181"/>
-      <c r="C25" s="181"/>
-      <c r="D25" s="181"/>
-      <c r="E25" s="181"/>
-      <c r="F25" s="181"/>
-      <c r="G25" s="181"/>
-      <c r="H25" s="181"/>
-      <c r="I25" s="181"/>
+      <c r="B25" s="194"/>
+      <c r="C25" s="194"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="194"/>
+      <c r="F25" s="194"/>
+      <c r="G25" s="194"/>
+      <c r="H25" s="194"/>
+      <c r="I25" s="194"/>
       <c r="J25" s="163"/>
       <c r="K25" s="152"/>
       <c r="L25" s="164"/>
       <c r="M25" s="152"/>
       <c r="N25" s="167"/>
       <c r="O25" s="166"/>
-      <c r="P25" s="174"/>
-      <c r="Q25" s="177"/>
-      <c r="R25" s="178"/>
+      <c r="P25" s="199"/>
+      <c r="Q25" s="202"/>
+      <c r="R25" s="203"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="1:19" ht="30" customHeight="1">
       <c r="A26" s="7"/>
-      <c r="B26" s="181"/>
-      <c r="C26" s="181"/>
-      <c r="D26" s="181"/>
-      <c r="E26" s="181"/>
-      <c r="F26" s="181"/>
-      <c r="G26" s="181"/>
-      <c r="H26" s="181"/>
-      <c r="I26" s="181"/>
+      <c r="B26" s="194"/>
+      <c r="C26" s="194"/>
+      <c r="D26" s="194"/>
+      <c r="E26" s="194"/>
+      <c r="F26" s="194"/>
+      <c r="G26" s="194"/>
+      <c r="H26" s="194"/>
+      <c r="I26" s="194"/>
       <c r="J26" s="165"/>
       <c r="K26" s="168"/>
       <c r="L26" s="152"/>
       <c r="M26" s="152"/>
       <c r="N26" s="167"/>
       <c r="O26" s="166"/>
-      <c r="P26" s="174"/>
-      <c r="Q26" s="177"/>
-      <c r="R26" s="178"/>
+      <c r="P26" s="199"/>
+      <c r="Q26" s="202"/>
+      <c r="R26" s="203"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="1:19" ht="30" customHeight="1">
       <c r="A27" s="7"/>
-      <c r="B27" s="181"/>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="181"/>
-      <c r="F27" s="181"/>
-      <c r="G27" s="181"/>
-      <c r="H27" s="181"/>
-      <c r="I27" s="181"/>
+      <c r="B27" s="194"/>
+      <c r="C27" s="194"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="194"/>
+      <c r="F27" s="194"/>
+      <c r="G27" s="194"/>
+      <c r="H27" s="194"/>
+      <c r="I27" s="194"/>
       <c r="J27" s="165"/>
       <c r="K27" s="168"/>
       <c r="L27" s="152"/>
       <c r="M27" s="152"/>
       <c r="N27" s="167"/>
       <c r="O27" s="166"/>
-      <c r="P27" s="174"/>
-      <c r="Q27" s="179"/>
-      <c r="R27" s="180"/>
+      <c r="P27" s="199"/>
+      <c r="Q27" s="204"/>
+      <c r="R27" s="205"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:19" ht="9.75" hidden="1" customHeight="1" thickBot="1">
@@ -3233,7 +3246,7 @@
     <row r="36" spans="1:19" ht="30" hidden="1" customHeight="1"/>
     <row r="37" spans="1:19" ht="30" hidden="1" customHeight="1"/>
     <row r="38" spans="1:19" ht="30" hidden="1" customHeight="1"/>
-    <row r="39" spans="1:19" ht="13.9" thickBot="1">
+    <row r="39" spans="1:19" ht="13.5" thickBot="1">
       <c r="A39" s="169"/>
       <c r="B39" s="170"/>
       <c r="C39" s="170"/>
@@ -3254,79 +3267,61 @@
       <c r="R39" s="170"/>
       <c r="S39" s="171"/>
     </row>
-    <row r="40" spans="1:19"/>
-    <row r="41" spans="1:19"/>
-    <row r="42" spans="1:19"/>
-    <row r="43" spans="1:19"/>
-    <row r="44" spans="1:19">
-      <c r="L44" s="172"/>
-      <c r="M44" s="172"/>
-      <c r="N44" s="172"/>
+    <row r="40" spans="1:19" ht="12.75"/>
+    <row r="41" spans="1:19" ht="12.75"/>
+    <row r="42" spans="1:19" ht="12.75"/>
+    <row r="43" spans="1:19" ht="12.75"/>
+    <row r="44" spans="1:19" ht="12.75">
+      <c r="L44" s="197"/>
+      <c r="M44" s="197"/>
+      <c r="N44" s="197"/>
     </row>
-    <row r="45" spans="1:19">
-      <c r="L45" s="172"/>
-      <c r="M45" s="172"/>
-      <c r="N45" s="172"/>
+    <row r="45" spans="1:19" ht="12.75">
+      <c r="L45" s="197"/>
+      <c r="M45" s="197"/>
+      <c r="N45" s="197"/>
     </row>
-    <row r="46" spans="1:19"/>
-    <row r="47" spans="1:19"/>
-    <row r="48" spans="1:19"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
+    <row r="46" spans="1:19" ht="12.75"/>
+    <row r="47" spans="1:19" ht="12.75"/>
+    <row r="48" spans="1:19" ht="12.75"/>
+    <row r="49" ht="12.75"/>
+    <row r="50" ht="12.75"/>
+    <row r="51" ht="12.75"/>
+    <row r="52" ht="12.75"/>
+    <row r="53" ht="12.75"/>
+    <row r="54" ht="12.75"/>
+    <row r="55" ht="12.75"/>
+    <row r="56" ht="12.75"/>
+    <row r="57" ht="12.75"/>
+    <row r="58" ht="12.75"/>
+    <row r="59" ht="12.75"/>
+    <row r="60" ht="12.75"/>
+    <row r="61" ht="12.75"/>
+    <row r="62" ht="12.75"/>
+    <row r="63" ht="12.75"/>
+    <row r="64" ht="12.75"/>
+    <row r="65" ht="12.75"/>
+    <row r="66" ht="12.75"/>
+    <row r="67" ht="12.75"/>
+    <row r="68" ht="12.75"/>
+    <row r="69" ht="12.75"/>
+    <row r="70" ht="12.75"/>
+    <row r="71" ht="12.75"/>
+    <row r="72" ht="12.75"/>
+    <row r="73" ht="12.75"/>
+    <row r="74" ht="12.75"/>
+    <row r="75" ht="12.75"/>
+    <row r="76" ht="12.75"/>
+    <row r="77" ht="12.75"/>
+    <row r="78" ht="12.75"/>
+    <row r="79" ht="12.75"/>
+    <row r="80" ht="12.75"/>
+    <row r="81" ht="12.75"/>
+    <row r="82" ht="12.75"/>
+    <row r="83" ht="12.75"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="27">
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="P17:P19"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="B22:I22"/>
     <mergeCell ref="L44:N45"/>
     <mergeCell ref="P23:P27"/>
     <mergeCell ref="Q23:R27"/>
@@ -3336,6 +3331,24 @@
     <mergeCell ref="B27:I27"/>
     <mergeCell ref="B23:I23"/>
     <mergeCell ref="M23:O23"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="P17:P19"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <conditionalFormatting sqref="Q23:R27">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -3382,15 +3395,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f813ab756c42af8af494d6605e22e37b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98d92101-24da-4498-9971-a24673344bd8" xmlns:ns3="dfa80de1-e9bb-4cf2-893d-d06220b3971a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="808c042e6474ee35eb4b0b0b71aaa865" ns2:_="" ns3:_="">
     <xsd:import namespace="98d92101-24da-4498-9971-a24673344bd8"/>
@@ -3567,14 +3571,49 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB127613-3E42-413C-AA19-20FDD7FDB721}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB127613-3E42-413C-AA19-20FDD7FDB721}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
+    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D42627D-2FD8-4CD0-813D-983EAA15F567}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E97D3F8-EB60-4F3F-861E-88C92BD29808}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="98d92101-24da-4498-9971-a24673344bd8"/>
+    <ds:schemaRef ds:uri="dfa80de1-e9bb-4cf2-893d-d06220b3971a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E97D3F8-EB60-4F3F-861E-88C92BD29808}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D42627D-2FD8-4CD0-813D-983EAA15F567}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
livrable Beta2 prêt (02.12.2022[08:33])
</commit_message>
<xml_diff>
--- a/documents/AutoEval_Dussault_Morgan.xlsx
+++ b/documents/AutoEval_Dussault_Morgan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg66hua\Documents\GitHub\Space-invader\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77E2315-8F5C-4BE8-B69F-4B71B46FE6EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3439B113-351E-4BBD-B822-AA0860DF0B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dussault_Morgan" sheetId="1" r:id="rId1"/>
@@ -1582,35 +1582,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1648,42 +1656,34 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2329,8 +2329,8 @@
   </sheetPr>
   <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="13.15" customHeight="1" zeroHeight="1"/>
@@ -2372,11 +2372,11 @@
       <c r="M1" s="4"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="172" t="s">
+      <c r="P1" s="196" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="172"/>
-      <c r="R1" s="172"/>
+      <c r="Q1" s="196"/>
+      <c r="R1" s="196"/>
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:23" ht="37.5" customHeight="1">
@@ -2464,14 +2464,14 @@
       <c r="M4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="173" t="str">
+      <c r="N4" s="197" t="str">
         <f>[1]Automation!F12</f>
         <v>29.8.2022 - 9.1.2023</v>
       </c>
-      <c r="O4" s="173"/>
-      <c r="P4" s="173"/>
-      <c r="Q4" s="173"/>
-      <c r="R4" s="173"/>
+      <c r="O4" s="197"/>
+      <c r="P4" s="197"/>
+      <c r="Q4" s="197"/>
+      <c r="R4" s="197"/>
       <c r="S4" s="27"/>
     </row>
     <row r="5" spans="1:23" s="28" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -2511,34 +2511,34 @@
     <row r="7" spans="1:23" s="50" customFormat="1" ht="70.150000000000006" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="49"/>
       <c r="D7" s="51"/>
-      <c r="E7" s="174" t="str">
+      <c r="E7" s="198" t="str">
         <f>[1]INDICATEURS!E7</f>
         <v>LARGEMENT ACQUIS
 5.5 ou 6.0</v>
       </c>
-      <c r="F7" s="175"/>
-      <c r="G7" s="175"/>
-      <c r="H7" s="176" t="str">
+      <c r="F7" s="199"/>
+      <c r="G7" s="199"/>
+      <c r="H7" s="200" t="str">
         <f>[1]INDICATEURS!H7</f>
         <v>SUFFISANT
 4.0, 4.5 ou 5.0</v>
       </c>
-      <c r="I7" s="177"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="178" t="str">
+      <c r="I7" s="201"/>
+      <c r="J7" s="201"/>
+      <c r="K7" s="202" t="str">
         <f>[1]INDICATEURS!K7</f>
         <v>INSUFFISANT
 2.5, 3.0 ou 3.5</v>
       </c>
-      <c r="L7" s="179"/>
-      <c r="M7" s="179"/>
-      <c r="N7" s="180" t="str">
+      <c r="L7" s="203"/>
+      <c r="M7" s="203"/>
+      <c r="N7" s="204" t="str">
         <f>[1]INDICATEURS!N7</f>
         <v>NON ACQUIS
 1.0, 1.5, ou 2.0</v>
       </c>
-      <c r="O7" s="181"/>
-      <c r="P7" s="181"/>
+      <c r="O7" s="205"/>
+      <c r="P7" s="205"/>
       <c r="Q7" s="52" t="str">
         <f>[1]INDICATEURS!Q7</f>
         <v>Coeff.</v>
@@ -2552,11 +2552,11 @@
     </row>
     <row r="8" spans="1:23" ht="100.15" customHeight="1" thickTop="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="182" t="str">
+      <c r="B8" s="184" t="str">
         <f>[1]INDICATEURS!B8</f>
         <v>COMPÉTENCES</v>
       </c>
-      <c r="C8" s="185" t="str">
+      <c r="C8" s="187" t="str">
         <f>[1]INDICATEURS!C8</f>
         <v>PROFESSIONNELLES</v>
       </c>
@@ -2581,7 +2581,9 @@
         <f>[1]INDICATEURS!I8</f>
         <v>Respecte les délais fixés avec un rythme normal</v>
       </c>
-      <c r="J8" s="62"/>
+      <c r="J8" s="62">
+        <v>4</v>
+      </c>
       <c r="K8" s="63" t="s">
         <v>9</v>
       </c>
@@ -2602,16 +2604,16 @@
         <f>[1]INDICATEURS!Q8</f>
         <v>1</v>
       </c>
-      <c r="R8" s="70" t="str">
+      <c r="R8" s="70">
         <f t="shared" ref="R8:R15" si="0">IF(COUNT(G8,J8,M8,P8)=0,"",IF(COUNT(G8,J8,M8,P8)&lt;&gt;1,"ERREUR",Q8*(G8+J8+M8+P8)))</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="S8" s="13"/>
     </row>
     <row r="9" spans="1:23" ht="100.15" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="183"/>
-      <c r="C9" s="186"/>
+      <c r="B9" s="185"/>
+      <c r="C9" s="188"/>
       <c r="D9" s="71" t="str">
         <f>[1]INDICATEURS!D9</f>
         <v>Conscience professionnelle
@@ -2633,7 +2635,9 @@
         <f>[1]INDICATEURS!I9</f>
         <v>Produit un travail utilisable, et transmissible, moyennant quelques retouches</v>
       </c>
-      <c r="J9" s="77"/>
+      <c r="J9" s="77">
+        <v>4.5</v>
+      </c>
       <c r="K9" s="78" t="s">
         <v>9</v>
       </c>
@@ -2654,16 +2658,16 @@
         <f>[1]INDICATEURS!Q9</f>
         <v>1</v>
       </c>
-      <c r="R9" s="85" t="str">
+      <c r="R9" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>4.5</v>
       </c>
       <c r="S9" s="13"/>
     </row>
     <row r="10" spans="1:23" ht="100.15" customHeight="1" thickBot="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="183"/>
-      <c r="C10" s="186"/>
+      <c r="B10" s="185"/>
+      <c r="C10" s="188"/>
       <c r="D10" s="71" t="str">
         <f>[1]INDICATEURS!D10</f>
         <v>Connaissances professionnelles
@@ -2685,7 +2689,9 @@
         <f>[1]INDICATEURS!I10</f>
         <v>Intègre relativement dans sa pratique les notions théoriques apprises</v>
       </c>
-      <c r="J10" s="89"/>
+      <c r="J10" s="89">
+        <v>5</v>
+      </c>
       <c r="K10" s="90" t="s">
         <v>9</v>
       </c>
@@ -2706,16 +2712,16 @@
         <f>[1]INDICATEURS!Q10</f>
         <v>1</v>
       </c>
-      <c r="R10" s="85" t="str">
+      <c r="R10" s="85">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="S10" s="13"/>
     </row>
     <row r="11" spans="1:23" ht="100.15" customHeight="1" thickTop="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="183"/>
-      <c r="C11" s="187" t="str">
+      <c r="B11" s="185"/>
+      <c r="C11" s="189" t="str">
         <f>[1]INDICATEURS!C11</f>
         <v>METHODOLOGIQUES</v>
       </c>
@@ -2739,7 +2745,9 @@
         <f>[1]INDICATEURS!I11</f>
         <v>Respecte à peu près les règles et processus de travail</v>
       </c>
-      <c r="J11" s="96"/>
+      <c r="J11" s="96">
+        <v>4.5</v>
+      </c>
       <c r="K11" s="63" t="s">
         <v>9</v>
       </c>
@@ -2760,16 +2768,16 @@
         <f>[1]INDICATEURS!Q11</f>
         <v>1</v>
       </c>
-      <c r="R11" s="101" t="str">
+      <c r="R11" s="101">
         <f t="shared" si="0"/>
-        <v/>
+        <v>4.5</v>
       </c>
       <c r="S11" s="13"/>
     </row>
     <row r="12" spans="1:23" ht="100.15" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="183"/>
-      <c r="C12" s="188"/>
+      <c r="B12" s="185"/>
+      <c r="C12" s="190"/>
       <c r="D12" s="102" t="str">
         <f>[1]INDICATEURS!D12</f>
         <v>Expression orale et écrite
@@ -2799,7 +2807,9 @@
         <f>[1]INDICATEURS!L12</f>
         <v>Pourrait utiliser plus, ou mieux, les différents moyens et outils de communication et de documentation</v>
       </c>
-      <c r="M12" s="111"/>
+      <c r="M12" s="111">
+        <v>3.5</v>
+      </c>
       <c r="N12" s="112" t="s">
         <v>9</v>
       </c>
@@ -2812,16 +2822,16 @@
         <f>[1]INDICATEURS!Q12</f>
         <v>1</v>
       </c>
-      <c r="R12" s="116" t="str">
+      <c r="R12" s="116">
         <f t="shared" si="0"/>
-        <v/>
+        <v>3.5</v>
       </c>
       <c r="S12" s="13"/>
     </row>
     <row r="13" spans="1:23" ht="100.15" customHeight="1" thickBot="1">
       <c r="A13" s="7"/>
-      <c r="B13" s="183"/>
-      <c r="C13" s="189"/>
+      <c r="B13" s="185"/>
+      <c r="C13" s="191"/>
       <c r="D13" s="117" t="str">
         <f>[1]INDICATEURS!D13</f>
         <v>Approche écologique et économique
@@ -2872,7 +2882,7 @@
     </row>
     <row r="14" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="7"/>
-      <c r="B14" s="183"/>
+      <c r="B14" s="185"/>
       <c r="C14" s="128" t="str">
         <f>[1]INDICATEURS!C14</f>
         <v>SOCIALES</v>
@@ -2898,7 +2908,9 @@
         <v>Maintien les bonnes relations
 et participe aux solutions</v>
       </c>
-      <c r="J14" s="130"/>
+      <c r="J14" s="130">
+        <v>5</v>
+      </c>
       <c r="K14" s="90" t="s">
         <v>9</v>
       </c>
@@ -2919,15 +2931,15 @@
         <f>[1]INDICATEURS!Q14</f>
         <v>1</v>
       </c>
-      <c r="R14" s="135" t="str">
+      <c r="R14" s="135">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="S14" s="13"/>
     </row>
     <row r="15" spans="1:23" ht="120" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="7"/>
-      <c r="B15" s="184"/>
+      <c r="B15" s="186"/>
       <c r="C15" s="128" t="str">
         <f>[1]INDICATEURS!C15</f>
         <v>PERSONNELLES</v>
@@ -2954,7 +2966,9 @@
         <f>[1]INDICATEURS!I15</f>
         <v>A parfois besoin d'aide (justifiée), fait ce qui est attendu de sa personne</v>
       </c>
-      <c r="J15" s="142"/>
+      <c r="J15" s="142">
+        <v>5</v>
+      </c>
       <c r="K15" s="143" t="s">
         <v>9</v>
       </c>
@@ -2975,9 +2989,9 @@
         <f>[1]INDICATEURS!Q15</f>
         <v>1</v>
       </c>
-      <c r="R15" s="135" t="str">
+      <c r="R15" s="135">
         <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="S15" s="13"/>
     </row>
@@ -2999,7 +3013,7 @@
       <c r="M17" s="151"/>
       <c r="N17" s="153"/>
       <c r="O17" s="154"/>
-      <c r="P17" s="190" t="s">
+      <c r="P17" s="192" t="s">
         <v>11</v>
       </c>
       <c r="Q17" s="155"/>
@@ -3015,43 +3029,45 @@
       <c r="M18" s="152"/>
       <c r="N18" s="152"/>
       <c r="O18" s="152"/>
-      <c r="P18" s="190"/>
+      <c r="P18" s="192"/>
       <c r="Q18" s="155"/>
       <c r="R18" s="155"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="1:19" ht="30" customHeight="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="191"/>
-      <c r="C19" s="191"/>
-      <c r="D19" s="191"/>
-      <c r="E19" s="191"/>
-      <c r="F19" s="191"/>
-      <c r="G19" s="191"/>
-      <c r="H19" s="191"/>
-      <c r="I19" s="191"/>
-      <c r="K19" s="192" t="s">
+      <c r="B19" s="193"/>
+      <c r="C19" s="193"/>
+      <c r="D19" s="193"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="193"/>
+      <c r="K19" s="194" t="s">
         <v>12</v>
       </c>
-      <c r="L19" s="192"/>
-      <c r="M19" s="193"/>
-      <c r="N19" s="193"/>
-      <c r="O19" s="193"/>
-      <c r="P19" s="190"/>
+      <c r="L19" s="194"/>
+      <c r="M19" s="195">
+        <v>44897</v>
+      </c>
+      <c r="N19" s="195"/>
+      <c r="O19" s="195"/>
+      <c r="P19" s="192"/>
       <c r="Q19" s="155"/>
       <c r="R19" s="155"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="1:19" ht="30" customHeight="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="194"/>
-      <c r="C20" s="194"/>
-      <c r="D20" s="194"/>
-      <c r="E20" s="194"/>
-      <c r="F20" s="194"/>
-      <c r="G20" s="194"/>
-      <c r="H20" s="194"/>
-      <c r="I20" s="194"/>
+      <c r="B20" s="181"/>
+      <c r="C20" s="181"/>
+      <c r="D20" s="181"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="181"/>
       <c r="K20" s="158"/>
       <c r="L20" s="158"/>
       <c r="M20" s="152"/>
@@ -3064,23 +3080,23 @@
     </row>
     <row r="21" spans="1:19" ht="30" customHeight="1">
       <c r="A21" s="7"/>
-      <c r="B21" s="194"/>
-      <c r="C21" s="194"/>
-      <c r="D21" s="194"/>
-      <c r="E21" s="194"/>
-      <c r="F21" s="194"/>
-      <c r="G21" s="194"/>
-      <c r="H21" s="194"/>
-      <c r="I21" s="194"/>
-      <c r="K21" s="195" t="s">
+      <c r="B21" s="181"/>
+      <c r="C21" s="181"/>
+      <c r="D21" s="181"/>
+      <c r="E21" s="181"/>
+      <c r="F21" s="181"/>
+      <c r="G21" s="181"/>
+      <c r="H21" s="181"/>
+      <c r="I21" s="181"/>
+      <c r="K21" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="L21" s="195"/>
-      <c r="M21" s="196" t="s">
+      <c r="L21" s="183"/>
+      <c r="M21" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="N21" s="196"/>
-      <c r="O21" s="196"/>
+      <c r="N21" s="182"/>
+      <c r="O21" s="182"/>
       <c r="P21" s="161"/>
       <c r="Q21" s="162"/>
       <c r="R21" s="162"/>
@@ -3088,14 +3104,14 @@
     </row>
     <row r="22" spans="1:19" ht="30" customHeight="1">
       <c r="A22" s="7"/>
-      <c r="B22" s="194"/>
-      <c r="C22" s="194"/>
-      <c r="D22" s="194"/>
-      <c r="E22" s="194"/>
-      <c r="F22" s="194"/>
-      <c r="G22" s="194"/>
-      <c r="H22" s="194"/>
-      <c r="I22" s="194"/>
+      <c r="B22" s="181"/>
+      <c r="C22" s="181"/>
+      <c r="D22" s="181"/>
+      <c r="E22" s="181"/>
+      <c r="F22" s="181"/>
+      <c r="G22" s="181"/>
+      <c r="H22" s="181"/>
+      <c r="I22" s="181"/>
       <c r="K22" s="152"/>
       <c r="L22" s="152"/>
       <c r="M22" s="152"/>
@@ -3107,112 +3123,112 @@
     </row>
     <row r="23" spans="1:19" ht="30" customHeight="1">
       <c r="A23" s="7"/>
-      <c r="B23" s="194"/>
-      <c r="C23" s="194"/>
-      <c r="D23" s="194"/>
-      <c r="E23" s="194"/>
-      <c r="F23" s="194"/>
-      <c r="G23" s="194"/>
-      <c r="H23" s="194"/>
-      <c r="I23" s="194"/>
+      <c r="B23" s="181"/>
+      <c r="C23" s="181"/>
+      <c r="D23" s="181"/>
+      <c r="E23" s="181"/>
+      <c r="F23" s="181"/>
+      <c r="G23" s="181"/>
+      <c r="H23" s="181"/>
+      <c r="I23" s="181"/>
       <c r="J23" s="163"/>
       <c r="K23" s="151" t="s">
         <v>14</v>
       </c>
       <c r="L23" s="164"/>
-      <c r="M23" s="196"/>
-      <c r="N23" s="196"/>
-      <c r="O23" s="196"/>
-      <c r="P23" s="198"/>
-      <c r="Q23" s="200" t="str">
+      <c r="M23" s="182"/>
+      <c r="N23" s="182"/>
+      <c r="O23" s="182"/>
+      <c r="P23" s="173"/>
+      <c r="Q23" s="175">
         <f>IF(COUNT(R8:R15)=8,MROUND(SUM(R8:R15)/SUM(Q8:Q15),0.5),"")</f>
-        <v/>
-      </c>
-      <c r="R23" s="201"/>
+        <v>4.5</v>
+      </c>
+      <c r="R23" s="176"/>
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:19" ht="30" customHeight="1">
       <c r="A24" s="7"/>
-      <c r="B24" s="194"/>
-      <c r="C24" s="194"/>
-      <c r="D24" s="194"/>
-      <c r="E24" s="194"/>
-      <c r="F24" s="194"/>
-      <c r="G24" s="194"/>
-      <c r="H24" s="194"/>
-      <c r="I24" s="194"/>
+      <c r="B24" s="181"/>
+      <c r="C24" s="181"/>
+      <c r="D24" s="181"/>
+      <c r="E24" s="181"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="181"/>
+      <c r="H24" s="181"/>
+      <c r="I24" s="181"/>
       <c r="J24" s="165"/>
       <c r="K24" s="152"/>
       <c r="L24" s="151"/>
       <c r="M24" s="151"/>
       <c r="N24" s="151"/>
       <c r="O24" s="166"/>
-      <c r="P24" s="199"/>
-      <c r="Q24" s="202"/>
-      <c r="R24" s="203"/>
+      <c r="P24" s="174"/>
+      <c r="Q24" s="177"/>
+      <c r="R24" s="178"/>
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="1:19" ht="28.5" customHeight="1">
       <c r="A25" s="7"/>
-      <c r="B25" s="194"/>
-      <c r="C25" s="194"/>
-      <c r="D25" s="194"/>
-      <c r="E25" s="194"/>
-      <c r="F25" s="194"/>
-      <c r="G25" s="194"/>
-      <c r="H25" s="194"/>
-      <c r="I25" s="194"/>
+      <c r="B25" s="181"/>
+      <c r="C25" s="181"/>
+      <c r="D25" s="181"/>
+      <c r="E25" s="181"/>
+      <c r="F25" s="181"/>
+      <c r="G25" s="181"/>
+      <c r="H25" s="181"/>
+      <c r="I25" s="181"/>
       <c r="J25" s="163"/>
       <c r="K25" s="152"/>
       <c r="L25" s="164"/>
       <c r="M25" s="152"/>
       <c r="N25" s="167"/>
       <c r="O25" s="166"/>
-      <c r="P25" s="199"/>
-      <c r="Q25" s="202"/>
-      <c r="R25" s="203"/>
+      <c r="P25" s="174"/>
+      <c r="Q25" s="177"/>
+      <c r="R25" s="178"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="1:19" ht="30" customHeight="1">
       <c r="A26" s="7"/>
-      <c r="B26" s="194"/>
-      <c r="C26" s="194"/>
-      <c r="D26" s="194"/>
-      <c r="E26" s="194"/>
-      <c r="F26" s="194"/>
-      <c r="G26" s="194"/>
-      <c r="H26" s="194"/>
-      <c r="I26" s="194"/>
+      <c r="B26" s="181"/>
+      <c r="C26" s="181"/>
+      <c r="D26" s="181"/>
+      <c r="E26" s="181"/>
+      <c r="F26" s="181"/>
+      <c r="G26" s="181"/>
+      <c r="H26" s="181"/>
+      <c r="I26" s="181"/>
       <c r="J26" s="165"/>
       <c r="K26" s="168"/>
       <c r="L26" s="152"/>
       <c r="M26" s="152"/>
       <c r="N26" s="167"/>
       <c r="O26" s="166"/>
-      <c r="P26" s="199"/>
-      <c r="Q26" s="202"/>
-      <c r="R26" s="203"/>
+      <c r="P26" s="174"/>
+      <c r="Q26" s="177"/>
+      <c r="R26" s="178"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="1:19" ht="30" customHeight="1">
       <c r="A27" s="7"/>
-      <c r="B27" s="194"/>
-      <c r="C27" s="194"/>
-      <c r="D27" s="194"/>
-      <c r="E27" s="194"/>
-      <c r="F27" s="194"/>
-      <c r="G27" s="194"/>
-      <c r="H27" s="194"/>
-      <c r="I27" s="194"/>
+      <c r="B27" s="181"/>
+      <c r="C27" s="181"/>
+      <c r="D27" s="181"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="181"/>
+      <c r="G27" s="181"/>
+      <c r="H27" s="181"/>
+      <c r="I27" s="181"/>
       <c r="J27" s="165"/>
       <c r="K27" s="168"/>
       <c r="L27" s="152"/>
       <c r="M27" s="152"/>
       <c r="N27" s="167"/>
       <c r="O27" s="166"/>
-      <c r="P27" s="199"/>
-      <c r="Q27" s="204"/>
-      <c r="R27" s="205"/>
+      <c r="P27" s="174"/>
+      <c r="Q27" s="179"/>
+      <c r="R27" s="180"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:19" ht="9.75" hidden="1" customHeight="1" thickBot="1">
@@ -3272,14 +3288,14 @@
     <row r="42" spans="1:19" ht="12.75"/>
     <row r="43" spans="1:19" ht="12.75"/>
     <row r="44" spans="1:19" ht="12.75">
-      <c r="L44" s="197"/>
-      <c r="M44" s="197"/>
-      <c r="N44" s="197"/>
+      <c r="L44" s="172"/>
+      <c r="M44" s="172"/>
+      <c r="N44" s="172"/>
     </row>
     <row r="45" spans="1:19" ht="12.75">
-      <c r="L45" s="197"/>
-      <c r="M45" s="197"/>
-      <c r="N45" s="197"/>
+      <c r="L45" s="172"/>
+      <c r="M45" s="172"/>
+      <c r="N45" s="172"/>
     </row>
     <row r="46" spans="1:19" ht="12.75"/>
     <row r="47" spans="1:19" ht="12.75"/>
@@ -3322,6 +3338,24 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="27">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="P17:P19"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="B22:I22"/>
     <mergeCell ref="L44:N45"/>
     <mergeCell ref="P23:P27"/>
     <mergeCell ref="Q23:R27"/>
@@ -3331,24 +3365,6 @@
     <mergeCell ref="B27:I27"/>
     <mergeCell ref="B23:I23"/>
     <mergeCell ref="M23:O23"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="P17:P19"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <conditionalFormatting sqref="Q23:R27">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -3395,6 +3411,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f813ab756c42af8af494d6605e22e37b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98d92101-24da-4498-9971-a24673344bd8" xmlns:ns3="dfa80de1-e9bb-4cf2-893d-d06220b3971a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="808c042e6474ee35eb4b0b0b71aaa865" ns2:_="" ns3:_="">
     <xsd:import namespace="98d92101-24da-4498-9971-a24673344bd8"/>
@@ -3571,15 +3596,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB127613-3E42-413C-AA19-20FDD7FDB721}">
   <ds:schemaRefs>
@@ -3592,6 +3608,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D42627D-2FD8-4CD0-813D-983EAA15F567}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E97D3F8-EB60-4F3F-861E-88C92BD29808}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3608,12 +3632,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D42627D-2FD8-4CD0-813D-983EAA15F567}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
réparation des problèmes + avance menu pause + avance tir (07.12.2022[16:25])
- stack overflow exception réglée
- classe menu bien implémentée (futurs modifications)
- réglage problème de synchronisation entre les différents déplacements
</commit_message>
<xml_diff>
--- a/documents/AutoEval_Dussault_Morgan.xlsx
+++ b/documents/AutoEval_Dussault_Morgan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg66hua\Documents\GitHub\Space-invader\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3439B113-351E-4BBD-B822-AA0860DF0B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7B1D72-3B7F-48BE-AB9B-31345F657FFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,11 +68,6 @@
     <t>Dates :</t>
   </si>
   <si>
-    <t>o
-o
-o</t>
-  </si>
-  <si>
     <t>Remarque(s) :</t>
   </si>
   <si>
@@ -89,6 +84,11 @@
   </si>
   <si>
     <t>Dussault Morgan</t>
+  </si>
+  <si>
+    <t>o
+o
+x</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1081,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1224,10 +1224,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1235,10 +1231,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1246,10 +1238,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1277,10 +1265,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1288,10 +1272,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1299,10 +1279,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1320,10 +1296,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1331,14 +1303,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1387,10 +1351,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1398,10 +1358,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1409,10 +1365,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1504,10 +1456,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1515,19 +1463,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="4" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="5" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1582,43 +1522,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1656,34 +1588,42 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2330,7 +2270,7 @@
   <dimension ref="A1:W83"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21:O21"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="13.15" customHeight="1" zeroHeight="1"/>
@@ -2372,11 +2312,11 @@
       <c r="M1" s="4"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="196" t="s">
+      <c r="P1" s="157" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="196"/>
-      <c r="R1" s="196"/>
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:23" ht="37.5" customHeight="1">
@@ -2464,14 +2404,14 @@
       <c r="M4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="197" t="str">
+      <c r="N4" s="158" t="str">
         <f>[1]Automation!F12</f>
         <v>29.8.2022 - 9.1.2023</v>
       </c>
-      <c r="O4" s="197"/>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="197"/>
-      <c r="R4" s="197"/>
+      <c r="O4" s="158"/>
+      <c r="P4" s="158"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
       <c r="S4" s="27"/>
     </row>
     <row r="5" spans="1:23" s="28" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -2511,34 +2451,34 @@
     <row r="7" spans="1:23" s="50" customFormat="1" ht="70.150000000000006" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="49"/>
       <c r="D7" s="51"/>
-      <c r="E7" s="198" t="str">
+      <c r="E7" s="159" t="str">
         <f>[1]INDICATEURS!E7</f>
         <v>LARGEMENT ACQUIS
 5.5 ou 6.0</v>
       </c>
-      <c r="F7" s="199"/>
-      <c r="G7" s="199"/>
-      <c r="H7" s="200" t="str">
+      <c r="F7" s="160"/>
+      <c r="G7" s="160"/>
+      <c r="H7" s="161" t="str">
         <f>[1]INDICATEURS!H7</f>
         <v>SUFFISANT
 4.0, 4.5 ou 5.0</v>
       </c>
-      <c r="I7" s="201"/>
-      <c r="J7" s="201"/>
-      <c r="K7" s="202" t="str">
+      <c r="I7" s="162"/>
+      <c r="J7" s="162"/>
+      <c r="K7" s="163" t="str">
         <f>[1]INDICATEURS!K7</f>
         <v>INSUFFISANT
 2.5, 3.0 ou 3.5</v>
       </c>
-      <c r="L7" s="203"/>
-      <c r="M7" s="203"/>
-      <c r="N7" s="204" t="str">
+      <c r="L7" s="164"/>
+      <c r="M7" s="164"/>
+      <c r="N7" s="165" t="str">
         <f>[1]INDICATEURS!N7</f>
         <v>NON ACQUIS
 1.0, 1.5, ou 2.0</v>
       </c>
-      <c r="O7" s="205"/>
-      <c r="P7" s="205"/>
+      <c r="O7" s="166"/>
+      <c r="P7" s="166"/>
       <c r="Q7" s="52" t="str">
         <f>[1]INDICATEURS!Q7</f>
         <v>Coeff.</v>
@@ -2550,13 +2490,13 @@
       <c r="S7" s="54"/>
       <c r="W7" s="55"/>
     </row>
-    <row r="8" spans="1:23" ht="100.15" customHeight="1" thickTop="1">
+    <row r="8" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="184" t="str">
+      <c r="B8" s="167" t="str">
         <f>[1]INDICATEURS!B8</f>
         <v>COMPÉTENCES</v>
       </c>
-      <c r="C8" s="187" t="str">
+      <c r="C8" s="170" t="str">
         <f>[1]INDICATEURS!C8</f>
         <v>PROFESSIONNELLES</v>
       </c>
@@ -2567,314 +2507,314 @@
 [Différence planification / réalisation]</v>
       </c>
       <c r="E8" s="57" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F8" s="58" t="str">
         <f>[1]INDICATEURS!F8</f>
         <v>Travaille rapidement et de façon optimale</v>
       </c>
       <c r="G8" s="59"/>
-      <c r="H8" s="60" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="61" t="str">
+      <c r="H8" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="60" t="str">
         <f>[1]INDICATEURS!I8</f>
         <v>Respecte les délais fixés avec un rythme normal</v>
       </c>
-      <c r="J8" s="62">
+      <c r="J8" s="61">
         <v>4</v>
       </c>
-      <c r="K8" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="64" t="str">
+      <c r="K8" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="62" t="str">
         <f>[1]INDICATEURS!L8</f>
         <v>Travaille lentement et ne respecte pas vraiment les délais</v>
       </c>
-      <c r="M8" s="65"/>
-      <c r="N8" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="67" t="str">
+      <c r="M8" s="63"/>
+      <c r="N8" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="O8" s="64" t="str">
         <f>[1]INDICATEURS!O8</f>
         <v>Travaille trop lentement et ne respecte pas assez les délais</v>
       </c>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="69">
+      <c r="P8" s="65"/>
+      <c r="Q8" s="66">
         <f>[1]INDICATEURS!Q8</f>
         <v>1</v>
       </c>
-      <c r="R8" s="70">
+      <c r="R8" s="67">
         <f t="shared" ref="R8:R15" si="0">IF(COUNT(G8,J8,M8,P8)=0,"",IF(COUNT(G8,J8,M8,P8)&lt;&gt;1,"ERREUR",Q8*(G8+J8+M8+P8)))</f>
         <v>4</v>
       </c>
       <c r="S8" s="13"/>
     </row>
-    <row r="9" spans="1:23" ht="100.15" customHeight="1">
+    <row r="9" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="185"/>
-      <c r="C9" s="188"/>
-      <c r="D9" s="71" t="str">
+      <c r="B9" s="168"/>
+      <c r="C9" s="171"/>
+      <c r="D9" s="68" t="str">
         <f>[1]INDICATEURS!D9</f>
         <v>Conscience professionnelle
 Qualité du travail
 [JDT, Commentaires]</v>
       </c>
-      <c r="E9" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="73" t="str">
+      <c r="E9" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="70" t="str">
         <f>[1]INDICATEURS!F9</f>
         <v>Produit un travail parfaitement utilisable et transmissible sans retouches</v>
       </c>
-      <c r="G9" s="74"/>
-      <c r="H9" s="75" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="76" t="str">
+      <c r="G9" s="71"/>
+      <c r="H9" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="72" t="str">
         <f>[1]INDICATEURS!I9</f>
         <v>Produit un travail utilisable, et transmissible, moyennant quelques retouches</v>
       </c>
-      <c r="J9" s="77">
+      <c r="J9" s="73">
         <v>4.5</v>
       </c>
-      <c r="K9" s="78" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="79" t="str">
+      <c r="K9" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="74" t="str">
         <f>[1]INDICATEURS!L9</f>
         <v>Produit un travail exigeant des corrections pour être utilisable</v>
       </c>
-      <c r="M9" s="80"/>
-      <c r="N9" s="81" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="82" t="str">
+      <c r="M9" s="75"/>
+      <c r="N9" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" s="76" t="str">
         <f>[1]INDICATEURS!O9</f>
         <v>Produit un travail qui est inutilisable</v>
       </c>
-      <c r="P9" s="83"/>
-      <c r="Q9" s="84">
+      <c r="P9" s="77"/>
+      <c r="Q9" s="78">
         <f>[1]INDICATEURS!Q9</f>
         <v>1</v>
       </c>
-      <c r="R9" s="85">
+      <c r="R9" s="79">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="S9" s="13"/>
     </row>
-    <row r="10" spans="1:23" ht="100.15" customHeight="1" thickBot="1">
+    <row r="10" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="185"/>
-      <c r="C10" s="188"/>
-      <c r="D10" s="71" t="str">
+      <c r="B10" s="168"/>
+      <c r="C10" s="171"/>
+      <c r="D10" s="68" t="str">
         <f>[1]INDICATEURS!D10</f>
         <v>Connaissances professionnelles
 Techniques enseignées
 [Types de variable, boucles, tableaux, algorithmes]</v>
       </c>
-      <c r="E10" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="73" t="str">
+      <c r="E10" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="70" t="str">
         <f>[1]INDICATEURS!F10</f>
         <v>Intègre totalement dans sa pratique les notions apprises</v>
       </c>
-      <c r="G10" s="74"/>
-      <c r="H10" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="88" t="str">
+      <c r="G10" s="71"/>
+      <c r="H10" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="81" t="str">
         <f>[1]INDICATEURS!I10</f>
         <v>Intègre relativement dans sa pratique les notions théoriques apprises</v>
       </c>
-      <c r="J10" s="89">
+      <c r="J10" s="82">
         <v>5</v>
       </c>
-      <c r="K10" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" s="79" t="str">
+      <c r="K10" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="74" t="str">
         <f>[1]INDICATEURS!L10</f>
         <v>Rencontre des difficultés dans sa pratique car a des lacunes dans les notions de bases</v>
       </c>
-      <c r="M10" s="80"/>
-      <c r="N10" s="91" t="s">
-        <v>9</v>
-      </c>
-      <c r="O10" s="82" t="str">
+      <c r="M10" s="75"/>
+      <c r="N10" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="76" t="str">
         <f>[1]INDICATEURS!O10</f>
         <v>Bloque régulièrement dans sa pratique par manques importants dans les notions de base</v>
       </c>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="84">
+      <c r="P10" s="77"/>
+      <c r="Q10" s="78">
         <f>[1]INDICATEURS!Q10</f>
         <v>1</v>
       </c>
-      <c r="R10" s="85">
+      <c r="R10" s="79">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="S10" s="13"/>
     </row>
-    <row r="11" spans="1:23" ht="100.15" customHeight="1" thickTop="1">
+    <row r="11" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="185"/>
-      <c r="C11" s="189" t="str">
+      <c r="B11" s="168"/>
+      <c r="C11" s="172" t="str">
         <f>[1]INDICATEURS!C11</f>
         <v>METHODOLOGIQUES</v>
       </c>
-      <c r="D11" s="92" t="str">
+      <c r="D11" s="83" t="str">
         <f>[1]INDICATEURS!D11</f>
         <v>Processus de travail
 [JDT à jour et au bon endroit, conventions, présence/ponctualité, livraison à temps]</v>
       </c>
       <c r="E11" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="93" t="str">
+        <v>15</v>
+      </c>
+      <c r="F11" s="84" t="str">
         <f>[1]INDICATEURS!F11</f>
         <v>Respecte parfaitement les règles et processus de travail</v>
       </c>
-      <c r="G11" s="94"/>
-      <c r="H11" s="60" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="95" t="str">
+      <c r="G11" s="85"/>
+      <c r="H11" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="86" t="str">
         <f>[1]INDICATEURS!I11</f>
         <v>Respecte à peu près les règles et processus de travail</v>
       </c>
-      <c r="J11" s="96">
+      <c r="J11" s="87">
         <v>4.5</v>
       </c>
-      <c r="K11" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="97" t="str">
+      <c r="K11" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="88" t="str">
         <f>[1]INDICATEURS!L11</f>
         <v>Devrait mieux respecter les règles et processus de travail</v>
       </c>
-      <c r="M11" s="98"/>
-      <c r="N11" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="O11" s="99" t="str">
+      <c r="M11" s="89"/>
+      <c r="N11" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="90" t="str">
         <f>[1]INDICATEURS!O11</f>
         <v>Ignore les règles et processus de travail</v>
       </c>
-      <c r="P11" s="100"/>
-      <c r="Q11" s="69">
+      <c r="P11" s="91"/>
+      <c r="Q11" s="66">
         <f>[1]INDICATEURS!Q11</f>
         <v>1</v>
       </c>
-      <c r="R11" s="101">
+      <c r="R11" s="92">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="S11" s="13"/>
     </row>
-    <row r="12" spans="1:23" ht="100.15" customHeight="1">
+    <row r="12" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="185"/>
-      <c r="C12" s="190"/>
-      <c r="D12" s="102" t="str">
+      <c r="B12" s="168"/>
+      <c r="C12" s="173"/>
+      <c r="D12" s="93" t="str">
         <f>[1]INDICATEURS!D12</f>
         <v>Expression orale et écrite
 Technique de présentation
 [Commentaires (Doxygen), Orthographe JDT, propreté du code]</v>
       </c>
-      <c r="E12" s="103" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="104" t="str">
+      <c r="E12" s="94" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="95" t="str">
         <f>[1]INDICATEURS!F12</f>
         <v>Maîtrise parfaitement les différents moyens et outils de communication et de documentation</v>
       </c>
-      <c r="G12" s="105"/>
-      <c r="H12" s="106" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="107" t="str">
+      <c r="G12" s="96"/>
+      <c r="H12" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="97" t="str">
         <f>[1]INDICATEURS!I12</f>
         <v>Utilise les différents moyens et outils de communication et de documentation</v>
       </c>
-      <c r="J12" s="108"/>
-      <c r="K12" s="109" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="110" t="str">
+      <c r="J12" s="98"/>
+      <c r="K12" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="99" t="str">
         <f>[1]INDICATEURS!L12</f>
         <v>Pourrait utiliser plus, ou mieux, les différents moyens et outils de communication et de documentation</v>
       </c>
-      <c r="M12" s="111">
+      <c r="M12" s="100">
         <v>3.5</v>
       </c>
-      <c r="N12" s="112" t="s">
-        <v>9</v>
-      </c>
-      <c r="O12" s="113" t="str">
+      <c r="N12" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="101" t="str">
         <f>[1]INDICATEURS!O12</f>
         <v>Ignore la plupart des moyens et outils de communication et de documentation</v>
       </c>
-      <c r="P12" s="114"/>
-      <c r="Q12" s="115">
+      <c r="P12" s="102"/>
+      <c r="Q12" s="103">
         <f>[1]INDICATEURS!Q12</f>
         <v>1</v>
       </c>
-      <c r="R12" s="116">
+      <c r="R12" s="104">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="S12" s="13"/>
     </row>
-    <row r="13" spans="1:23" ht="100.15" customHeight="1" thickBot="1">
+    <row r="13" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="7"/>
-      <c r="B13" s="185"/>
-      <c r="C13" s="191"/>
-      <c r="D13" s="117" t="str">
+      <c r="B13" s="168"/>
+      <c r="C13" s="174"/>
+      <c r="D13" s="105" t="str">
         <f>[1]INDICATEURS!D13</f>
         <v>Approche écologique et économique
 [Ecran/Multiprise, Moteur de recherche Ecosia, Utilisation mémoire/CPU]</v>
       </c>
-      <c r="E13" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="118" t="str">
+      <c r="E13" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="106" t="str">
         <f>[1]INDICATEURS!F13</f>
         <v>Recourt systématiquement aux technologies et moyens qui ménagent les ressources et les coûts</v>
       </c>
-      <c r="G13" s="119"/>
-      <c r="H13" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="120" t="str">
+      <c r="G13" s="107"/>
+      <c r="H13" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="108" t="str">
         <f>[1]INDICATEURS!I13</f>
         <v>Utilise les technologies et moyens qui ménagent les ressources et les coûts</v>
       </c>
-      <c r="J13" s="121">
+      <c r="J13" s="109">
         <v>5</v>
       </c>
-      <c r="K13" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="122" t="str">
+      <c r="K13" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="110" t="str">
         <f>[1]INDICATEURS!L13</f>
         <v>Devrait mieux utiliser les technologies et moyens qui ménagent les ressources et les coûts</v>
       </c>
-      <c r="M13" s="123"/>
-      <c r="N13" s="91" t="s">
-        <v>9</v>
-      </c>
-      <c r="O13" s="124" t="str">
+      <c r="M13" s="111"/>
+      <c r="N13" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" s="112" t="str">
         <f>[1]INDICATEURS!O13</f>
         <v>Ignore les technologies et moyens qui ménagent les ressources et les coûts</v>
       </c>
-      <c r="P13" s="125"/>
-      <c r="Q13" s="126">
+      <c r="P13" s="113"/>
+      <c r="Q13" s="114">
         <v>0</v>
       </c>
-      <c r="R13" s="127">
+      <c r="R13" s="115">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2882,56 +2822,56 @@
     </row>
     <row r="14" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="7"/>
-      <c r="B14" s="185"/>
-      <c r="C14" s="128" t="str">
+      <c r="B14" s="168"/>
+      <c r="C14" s="116" t="str">
         <f>[1]INDICATEURS!C14</f>
         <v>SOCIALES</v>
       </c>
-      <c r="D14" s="117" t="str">
+      <c r="D14" s="105" t="str">
         <f>[1]INDICATEURS!D14</f>
         <v>Aptitude au travail en équipe Gestion des conflits Communication
 [A l'écoute de soi et des autres, soutient le calme plutôt que le conflit]</v>
       </c>
-      <c r="E14" s="86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="118" t="str">
+      <c r="E14" s="80" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="106" t="str">
         <f>[1]INDICATEURS!F14</f>
         <v>Influence positivement le groupe, manifeste un esprit entreprenant, constructif et cherche des solutions</v>
       </c>
-      <c r="G14" s="119"/>
-      <c r="H14" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="129" t="str">
+      <c r="G14" s="107"/>
+      <c r="H14" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="117" t="str">
         <f>[1]INDICATEURS!I14</f>
         <v>Maintien les bonnes relations
 et participe aux solutions</v>
       </c>
-      <c r="J14" s="130">
+      <c r="J14" s="118">
         <v>5</v>
       </c>
-      <c r="K14" s="90" t="s">
-        <v>9</v>
-      </c>
-      <c r="L14" s="131" t="str">
+      <c r="K14" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="119" t="str">
         <f>[1]INDICATEURS!L14</f>
         <v>Perturbe parfois le bon fonctionnement du groupe, réagit de manière irréfléchie et/ou disproportionnée</v>
       </c>
-      <c r="M14" s="132"/>
-      <c r="N14" s="91" t="s">
-        <v>9</v>
-      </c>
-      <c r="O14" s="133" t="str">
+      <c r="M14" s="120"/>
+      <c r="N14" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="121" t="str">
         <f>[1]INDICATEURS!O14</f>
         <v xml:space="preserve">Se comporte socialement de manière irrespectueuse </v>
       </c>
-      <c r="P14" s="134"/>
-      <c r="Q14" s="126">
+      <c r="P14" s="122"/>
+      <c r="Q14" s="114">
         <f>[1]INDICATEURS!Q14</f>
         <v>1</v>
       </c>
-      <c r="R14" s="135">
+      <c r="R14" s="123">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2939,57 +2879,57 @@
     </row>
     <row r="15" spans="1:23" ht="120" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="7"/>
-      <c r="B15" s="186"/>
-      <c r="C15" s="128" t="str">
+      <c r="B15" s="169"/>
+      <c r="C15" s="116" t="str">
         <f>[1]INDICATEURS!C15</f>
         <v>PERSONNELLES</v>
       </c>
-      <c r="D15" s="136" t="str">
+      <c r="D15" s="124" t="str">
         <f>[1]INDICATEURS!D15</f>
         <v>Autonomie
 Attitude face au travail
 Faculté d'apprendre
 [Essayer 15m avant de poser une question...]</v>
       </c>
-      <c r="E15" s="137" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="138" t="str">
+      <c r="E15" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="126" t="str">
         <f>[1]INDICATEURS!F15</f>
         <v>Est indépendant, entreprenant, et s'adapte facilement aux changements</v>
       </c>
-      <c r="G15" s="139"/>
-      <c r="H15" s="140" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="141" t="str">
+      <c r="G15" s="127"/>
+      <c r="H15" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="128" t="str">
         <f>[1]INDICATEURS!I15</f>
         <v>A parfois besoin d'aide (justifiée), fait ce qui est attendu de sa personne</v>
       </c>
-      <c r="J15" s="142">
+      <c r="J15" s="129">
         <v>5</v>
       </c>
-      <c r="K15" s="143" t="s">
-        <v>9</v>
-      </c>
-      <c r="L15" s="144" t="str">
+      <c r="K15" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="130" t="str">
         <f>[1]INDICATEURS!L15</f>
         <v>A souvent besoin d'aide, minimise ses erreurs et subit les changements</v>
       </c>
-      <c r="M15" s="145"/>
-      <c r="N15" s="146" t="s">
-        <v>9</v>
-      </c>
-      <c r="O15" s="147" t="str">
+      <c r="M15" s="131"/>
+      <c r="N15" s="125" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15" s="132" t="str">
         <f>[1]INDICATEURS!O15</f>
         <v>Est trop dépendant des autres, nie ses erreurs et est inapte aux changements</v>
       </c>
-      <c r="P15" s="148"/>
-      <c r="Q15" s="126">
+      <c r="P15" s="133"/>
+      <c r="Q15" s="114">
         <f>[1]INDICATEURS!Q15</f>
         <v>1</v>
       </c>
-      <c r="R15" s="135">
+      <c r="R15" s="123">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2997,260 +2937,260 @@
     </row>
     <row r="16" spans="1:23" ht="5.0999999999999996" customHeight="1" thickTop="1">
       <c r="A16" s="7"/>
-      <c r="L16" s="149"/>
-      <c r="O16" s="149"/>
-      <c r="P16" s="149"/>
-      <c r="Q16" s="150"/>
+      <c r="L16" s="134"/>
+      <c r="O16" s="134"/>
+      <c r="P16" s="134"/>
+      <c r="Q16" s="135"/>
       <c r="S16" s="13"/>
     </row>
     <row r="17" spans="1:19" ht="25.5" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="151" t="s">
+      <c r="B17" s="136" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="137"/>
+      <c r="L17" s="137"/>
+      <c r="M17" s="136"/>
+      <c r="N17" s="138"/>
+      <c r="O17" s="139"/>
+      <c r="P17" s="175" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="152"/>
-      <c r="L17" s="152"/>
-      <c r="M17" s="151"/>
-      <c r="N17" s="153"/>
-      <c r="O17" s="154"/>
-      <c r="P17" s="192" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q17" s="155"/>
-      <c r="R17" s="155"/>
+      <c r="Q17" s="140"/>
+      <c r="R17" s="140"/>
       <c r="S17" s="13"/>
     </row>
     <row r="18" spans="1:19" ht="5.0999999999999996" customHeight="1">
       <c r="A18" s="7"/>
-      <c r="F18" s="156"/>
-      <c r="H18" s="157"/>
-      <c r="K18" s="152"/>
-      <c r="L18" s="152"/>
-      <c r="M18" s="152"/>
-      <c r="N18" s="152"/>
-      <c r="O18" s="152"/>
-      <c r="P18" s="192"/>
-      <c r="Q18" s="155"/>
-      <c r="R18" s="155"/>
+      <c r="F18" s="141"/>
+      <c r="H18" s="142"/>
+      <c r="K18" s="137"/>
+      <c r="L18" s="137"/>
+      <c r="M18" s="137"/>
+      <c r="N18" s="137"/>
+      <c r="O18" s="137"/>
+      <c r="P18" s="175"/>
+      <c r="Q18" s="140"/>
+      <c r="R18" s="140"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="1:19" ht="30" customHeight="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="193"/>
-      <c r="C19" s="193"/>
-      <c r="D19" s="193"/>
-      <c r="E19" s="193"/>
-      <c r="F19" s="193"/>
-      <c r="G19" s="193"/>
-      <c r="H19" s="193"/>
-      <c r="I19" s="193"/>
-      <c r="K19" s="194" t="s">
-        <v>12</v>
-      </c>
-      <c r="L19" s="194"/>
-      <c r="M19" s="195">
+      <c r="B19" s="176"/>
+      <c r="C19" s="176"/>
+      <c r="D19" s="176"/>
+      <c r="E19" s="176"/>
+      <c r="F19" s="176"/>
+      <c r="G19" s="176"/>
+      <c r="H19" s="176"/>
+      <c r="I19" s="176"/>
+      <c r="K19" s="177" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="177"/>
+      <c r="M19" s="178">
         <v>44897</v>
       </c>
-      <c r="N19" s="195"/>
-      <c r="O19" s="195"/>
-      <c r="P19" s="192"/>
-      <c r="Q19" s="155"/>
-      <c r="R19" s="155"/>
+      <c r="N19" s="178"/>
+      <c r="O19" s="178"/>
+      <c r="P19" s="175"/>
+      <c r="Q19" s="140"/>
+      <c r="R19" s="140"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="1:19" ht="30" customHeight="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="181"/>
-      <c r="C20" s="181"/>
-      <c r="D20" s="181"/>
-      <c r="E20" s="181"/>
-      <c r="F20" s="181"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="181"/>
-      <c r="K20" s="158"/>
-      <c r="L20" s="158"/>
-      <c r="M20" s="152"/>
-      <c r="N20" s="152"/>
-      <c r="O20" s="152"/>
-      <c r="P20" s="159"/>
-      <c r="Q20" s="160"/>
-      <c r="R20" s="155"/>
+      <c r="B20" s="179"/>
+      <c r="C20" s="179"/>
+      <c r="D20" s="179"/>
+      <c r="E20" s="179"/>
+      <c r="F20" s="179"/>
+      <c r="G20" s="179"/>
+      <c r="H20" s="179"/>
+      <c r="I20" s="179"/>
+      <c r="K20" s="143"/>
+      <c r="L20" s="143"/>
+      <c r="M20" s="137"/>
+      <c r="N20" s="137"/>
+      <c r="O20" s="137"/>
+      <c r="P20" s="144"/>
+      <c r="Q20" s="145"/>
+      <c r="R20" s="140"/>
       <c r="S20" s="13"/>
     </row>
     <row r="21" spans="1:19" ht="30" customHeight="1">
       <c r="A21" s="7"/>
-      <c r="B21" s="181"/>
-      <c r="C21" s="181"/>
-      <c r="D21" s="181"/>
-      <c r="E21" s="181"/>
-      <c r="F21" s="181"/>
-      <c r="G21" s="181"/>
-      <c r="H21" s="181"/>
-      <c r="I21" s="181"/>
-      <c r="K21" s="183" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" s="183"/>
-      <c r="M21" s="182" t="s">
-        <v>15</v>
-      </c>
-      <c r="N21" s="182"/>
-      <c r="O21" s="182"/>
-      <c r="P21" s="161"/>
-      <c r="Q21" s="162"/>
-      <c r="R21" s="162"/>
+      <c r="B21" s="179"/>
+      <c r="C21" s="179"/>
+      <c r="D21" s="179"/>
+      <c r="E21" s="179"/>
+      <c r="F21" s="179"/>
+      <c r="G21" s="179"/>
+      <c r="H21" s="179"/>
+      <c r="I21" s="179"/>
+      <c r="K21" s="180" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="180"/>
+      <c r="M21" s="181" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" s="181"/>
+      <c r="O21" s="181"/>
+      <c r="P21" s="146"/>
+      <c r="Q21" s="147"/>
+      <c r="R21" s="147"/>
       <c r="S21" s="13"/>
     </row>
     <row r="22" spans="1:19" ht="30" customHeight="1">
       <c r="A22" s="7"/>
-      <c r="B22" s="181"/>
-      <c r="C22" s="181"/>
-      <c r="D22" s="181"/>
-      <c r="E22" s="181"/>
-      <c r="F22" s="181"/>
-      <c r="G22" s="181"/>
-      <c r="H22" s="181"/>
-      <c r="I22" s="181"/>
-      <c r="K22" s="152"/>
-      <c r="L22" s="152"/>
-      <c r="M22" s="152"/>
-      <c r="N22" s="152"/>
-      <c r="O22" s="152"/>
-      <c r="P22" s="161"/>
-      <c r="Q22" s="161"/>
+      <c r="B22" s="179"/>
+      <c r="C22" s="179"/>
+      <c r="D22" s="179"/>
+      <c r="E22" s="179"/>
+      <c r="F22" s="179"/>
+      <c r="G22" s="179"/>
+      <c r="H22" s="179"/>
+      <c r="I22" s="179"/>
+      <c r="K22" s="137"/>
+      <c r="L22" s="137"/>
+      <c r="M22" s="137"/>
+      <c r="N22" s="137"/>
+      <c r="O22" s="137"/>
+      <c r="P22" s="146"/>
+      <c r="Q22" s="146"/>
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="1:19" ht="30" customHeight="1">
       <c r="A23" s="7"/>
-      <c r="B23" s="181"/>
-      <c r="C23" s="181"/>
-      <c r="D23" s="181"/>
-      <c r="E23" s="181"/>
-      <c r="F23" s="181"/>
-      <c r="G23" s="181"/>
-      <c r="H23" s="181"/>
-      <c r="I23" s="181"/>
-      <c r="J23" s="163"/>
-      <c r="K23" s="151" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="164"/>
-      <c r="M23" s="182"/>
-      <c r="N23" s="182"/>
-      <c r="O23" s="182"/>
-      <c r="P23" s="173"/>
-      <c r="Q23" s="175">
+      <c r="B23" s="179"/>
+      <c r="C23" s="179"/>
+      <c r="D23" s="179"/>
+      <c r="E23" s="179"/>
+      <c r="F23" s="179"/>
+      <c r="G23" s="179"/>
+      <c r="H23" s="179"/>
+      <c r="I23" s="179"/>
+      <c r="J23" s="148"/>
+      <c r="K23" s="136" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="149"/>
+      <c r="M23" s="181"/>
+      <c r="N23" s="181"/>
+      <c r="O23" s="181"/>
+      <c r="P23" s="183"/>
+      <c r="Q23" s="185">
         <f>IF(COUNT(R8:R15)=8,MROUND(SUM(R8:R15)/SUM(Q8:Q15),0.5),"")</f>
         <v>4.5</v>
       </c>
-      <c r="R23" s="176"/>
+      <c r="R23" s="186"/>
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:19" ht="30" customHeight="1">
       <c r="A24" s="7"/>
-      <c r="B24" s="181"/>
-      <c r="C24" s="181"/>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="181"/>
-      <c r="J24" s="165"/>
-      <c r="K24" s="152"/>
-      <c r="L24" s="151"/>
-      <c r="M24" s="151"/>
-      <c r="N24" s="151"/>
-      <c r="O24" s="166"/>
-      <c r="P24" s="174"/>
-      <c r="Q24" s="177"/>
-      <c r="R24" s="178"/>
+      <c r="B24" s="179"/>
+      <c r="C24" s="179"/>
+      <c r="D24" s="179"/>
+      <c r="E24" s="179"/>
+      <c r="F24" s="179"/>
+      <c r="G24" s="179"/>
+      <c r="H24" s="179"/>
+      <c r="I24" s="179"/>
+      <c r="J24" s="150"/>
+      <c r="K24" s="137"/>
+      <c r="L24" s="136"/>
+      <c r="M24" s="136"/>
+      <c r="N24" s="136"/>
+      <c r="O24" s="151"/>
+      <c r="P24" s="184"/>
+      <c r="Q24" s="187"/>
+      <c r="R24" s="188"/>
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="1:19" ht="28.5" customHeight="1">
       <c r="A25" s="7"/>
-      <c r="B25" s="181"/>
-      <c r="C25" s="181"/>
-      <c r="D25" s="181"/>
-      <c r="E25" s="181"/>
-      <c r="F25" s="181"/>
-      <c r="G25" s="181"/>
-      <c r="H25" s="181"/>
-      <c r="I25" s="181"/>
-      <c r="J25" s="163"/>
-      <c r="K25" s="152"/>
-      <c r="L25" s="164"/>
-      <c r="M25" s="152"/>
-      <c r="N25" s="167"/>
-      <c r="O25" s="166"/>
-      <c r="P25" s="174"/>
-      <c r="Q25" s="177"/>
-      <c r="R25" s="178"/>
+      <c r="B25" s="179"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="179"/>
+      <c r="E25" s="179"/>
+      <c r="F25" s="179"/>
+      <c r="G25" s="179"/>
+      <c r="H25" s="179"/>
+      <c r="I25" s="179"/>
+      <c r="J25" s="148"/>
+      <c r="K25" s="137"/>
+      <c r="L25" s="149"/>
+      <c r="M25" s="137"/>
+      <c r="N25" s="152"/>
+      <c r="O25" s="151"/>
+      <c r="P25" s="184"/>
+      <c r="Q25" s="187"/>
+      <c r="R25" s="188"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="1:19" ht="30" customHeight="1">
       <c r="A26" s="7"/>
-      <c r="B26" s="181"/>
-      <c r="C26" s="181"/>
-      <c r="D26" s="181"/>
-      <c r="E26" s="181"/>
-      <c r="F26" s="181"/>
-      <c r="G26" s="181"/>
-      <c r="H26" s="181"/>
-      <c r="I26" s="181"/>
-      <c r="J26" s="165"/>
-      <c r="K26" s="168"/>
-      <c r="L26" s="152"/>
-      <c r="M26" s="152"/>
-      <c r="N26" s="167"/>
-      <c r="O26" s="166"/>
-      <c r="P26" s="174"/>
-      <c r="Q26" s="177"/>
-      <c r="R26" s="178"/>
+      <c r="B26" s="179"/>
+      <c r="C26" s="179"/>
+      <c r="D26" s="179"/>
+      <c r="E26" s="179"/>
+      <c r="F26" s="179"/>
+      <c r="G26" s="179"/>
+      <c r="H26" s="179"/>
+      <c r="I26" s="179"/>
+      <c r="J26" s="150"/>
+      <c r="K26" s="153"/>
+      <c r="L26" s="137"/>
+      <c r="M26" s="137"/>
+      <c r="N26" s="152"/>
+      <c r="O26" s="151"/>
+      <c r="P26" s="184"/>
+      <c r="Q26" s="187"/>
+      <c r="R26" s="188"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="1:19" ht="30" customHeight="1">
       <c r="A27" s="7"/>
-      <c r="B27" s="181"/>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="181"/>
-      <c r="F27" s="181"/>
-      <c r="G27" s="181"/>
-      <c r="H27" s="181"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="165"/>
-      <c r="K27" s="168"/>
-      <c r="L27" s="152"/>
-      <c r="M27" s="152"/>
-      <c r="N27" s="167"/>
-      <c r="O27" s="166"/>
-      <c r="P27" s="174"/>
-      <c r="Q27" s="179"/>
-      <c r="R27" s="180"/>
+      <c r="B27" s="179"/>
+      <c r="C27" s="179"/>
+      <c r="D27" s="179"/>
+      <c r="E27" s="179"/>
+      <c r="F27" s="179"/>
+      <c r="G27" s="179"/>
+      <c r="H27" s="179"/>
+      <c r="I27" s="179"/>
+      <c r="J27" s="150"/>
+      <c r="K27" s="153"/>
+      <c r="L27" s="137"/>
+      <c r="M27" s="137"/>
+      <c r="N27" s="152"/>
+      <c r="O27" s="151"/>
+      <c r="P27" s="184"/>
+      <c r="Q27" s="189"/>
+      <c r="R27" s="190"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:19" ht="9.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="A28" s="169"/>
-      <c r="B28" s="170"/>
-      <c r="C28" s="170"/>
-      <c r="D28" s="170"/>
-      <c r="E28" s="170"/>
-      <c r="F28" s="170"/>
-      <c r="G28" s="170"/>
-      <c r="H28" s="170"/>
-      <c r="I28" s="170"/>
-      <c r="J28" s="170"/>
-      <c r="K28" s="170"/>
-      <c r="L28" s="170"/>
-      <c r="M28" s="170"/>
-      <c r="N28" s="170"/>
-      <c r="O28" s="170"/>
-      <c r="P28" s="170"/>
-      <c r="Q28" s="170"/>
-      <c r="R28" s="170"/>
-      <c r="S28" s="171"/>
+      <c r="A28" s="154"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="155"/>
+      <c r="L28" s="155"/>
+      <c r="M28" s="155"/>
+      <c r="N28" s="155"/>
+      <c r="O28" s="155"/>
+      <c r="P28" s="155"/>
+      <c r="Q28" s="155"/>
+      <c r="R28" s="155"/>
+      <c r="S28" s="156"/>
     </row>
     <row r="29" spans="1:19" ht="0.75" hidden="1" customHeight="1"/>
     <row r="30" spans="1:19" ht="9.9499999999999993" hidden="1" customHeight="1"/>
@@ -3263,39 +3203,39 @@
     <row r="37" spans="1:19" ht="30" hidden="1" customHeight="1"/>
     <row r="38" spans="1:19" ht="30" hidden="1" customHeight="1"/>
     <row r="39" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A39" s="169"/>
-      <c r="B39" s="170"/>
-      <c r="C39" s="170"/>
-      <c r="D39" s="170"/>
-      <c r="E39" s="170"/>
-      <c r="F39" s="170"/>
-      <c r="G39" s="170"/>
-      <c r="H39" s="170"/>
-      <c r="I39" s="170"/>
-      <c r="J39" s="170"/>
-      <c r="K39" s="170"/>
-      <c r="L39" s="170"/>
-      <c r="M39" s="170"/>
-      <c r="N39" s="170"/>
-      <c r="O39" s="170"/>
-      <c r="P39" s="170"/>
-      <c r="Q39" s="170"/>
-      <c r="R39" s="170"/>
-      <c r="S39" s="171"/>
+      <c r="A39" s="154"/>
+      <c r="B39" s="155"/>
+      <c r="C39" s="155"/>
+      <c r="D39" s="155"/>
+      <c r="E39" s="155"/>
+      <c r="F39" s="155"/>
+      <c r="G39" s="155"/>
+      <c r="H39" s="155"/>
+      <c r="I39" s="155"/>
+      <c r="J39" s="155"/>
+      <c r="K39" s="155"/>
+      <c r="L39" s="155"/>
+      <c r="M39" s="155"/>
+      <c r="N39" s="155"/>
+      <c r="O39" s="155"/>
+      <c r="P39" s="155"/>
+      <c r="Q39" s="155"/>
+      <c r="R39" s="155"/>
+      <c r="S39" s="156"/>
     </row>
     <row r="40" spans="1:19" ht="12.75"/>
     <row r="41" spans="1:19" ht="12.75"/>
     <row r="42" spans="1:19" ht="12.75"/>
     <row r="43" spans="1:19" ht="12.75"/>
     <row r="44" spans="1:19" ht="12.75">
-      <c r="L44" s="172"/>
-      <c r="M44" s="172"/>
-      <c r="N44" s="172"/>
+      <c r="L44" s="182"/>
+      <c r="M44" s="182"/>
+      <c r="N44" s="182"/>
     </row>
     <row r="45" spans="1:19" ht="12.75">
-      <c r="L45" s="172"/>
-      <c r="M45" s="172"/>
-      <c r="N45" s="172"/>
+      <c r="L45" s="182"/>
+      <c r="M45" s="182"/>
+      <c r="N45" s="182"/>
     </row>
     <row r="46" spans="1:19" ht="12.75"/>
     <row r="47" spans="1:19" ht="12.75"/>
@@ -3338,24 +3278,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="27">
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="P17:P19"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="B22:I22"/>
     <mergeCell ref="L44:N45"/>
     <mergeCell ref="P23:P27"/>
     <mergeCell ref="Q23:R27"/>
@@ -3365,6 +3287,24 @@
     <mergeCell ref="B27:I27"/>
     <mergeCell ref="B23:I23"/>
     <mergeCell ref="M23:O23"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="P17:P19"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <conditionalFormatting sqref="Q23:R27">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -3411,15 +3351,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f813ab756c42af8af494d6605e22e37b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98d92101-24da-4498-9971-a24673344bd8" xmlns:ns3="dfa80de1-e9bb-4cf2-893d-d06220b3971a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="808c042e6474ee35eb4b0b0b71aaa865" ns2:_="" ns3:_="">
     <xsd:import namespace="98d92101-24da-4498-9971-a24673344bd8"/>
@@ -3596,6 +3527,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB127613-3E42-413C-AA19-20FDD7FDB721}">
   <ds:schemaRefs>
@@ -3608,14 +3548,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D42627D-2FD8-4CD0-813D-983EAA15F567}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E97D3F8-EB60-4F3F-861E-88C92BD29808}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3632,4 +3564,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D42627D-2FD8-4CD0-813D-983EAA15F567}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ajout de l'auto évaluation
</commit_message>
<xml_diff>
--- a/documents/AutoEval_Dussault_Morgan.xlsx
+++ b/documents/AutoEval_Dussault_Morgan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg66hua\Documents\GitHub\Space-invader\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7B1D72-3B7F-48BE-AB9B-31345F657FFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB2D522-2015-4D4E-9DF4-80D91D29C7A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dussault_Morgan" sheetId="1" r:id="rId1"/>
@@ -1522,35 +1522,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1588,42 +1596,34 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="53" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2270,7 +2270,7 @@
   <dimension ref="A1:W83"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="13.15" customHeight="1" zeroHeight="1"/>
@@ -2312,11 +2312,11 @@
       <c r="M1" s="4"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="157" t="s">
+      <c r="P1" s="181" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="157"/>
-      <c r="R1" s="157"/>
+      <c r="Q1" s="181"/>
+      <c r="R1" s="181"/>
       <c r="S1" s="5"/>
     </row>
     <row r="2" spans="1:23" ht="37.5" customHeight="1">
@@ -2404,14 +2404,14 @@
       <c r="M4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="158" t="str">
+      <c r="N4" s="182" t="str">
         <f>[1]Automation!F12</f>
         <v>29.8.2022 - 9.1.2023</v>
       </c>
-      <c r="O4" s="158"/>
-      <c r="P4" s="158"/>
-      <c r="Q4" s="158"/>
-      <c r="R4" s="158"/>
+      <c r="O4" s="182"/>
+      <c r="P4" s="182"/>
+      <c r="Q4" s="182"/>
+      <c r="R4" s="182"/>
       <c r="S4" s="27"/>
     </row>
     <row r="5" spans="1:23" s="28" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -2451,34 +2451,34 @@
     <row r="7" spans="1:23" s="50" customFormat="1" ht="70.150000000000006" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="49"/>
       <c r="D7" s="51"/>
-      <c r="E7" s="159" t="str">
+      <c r="E7" s="183" t="str">
         <f>[1]INDICATEURS!E7</f>
         <v>LARGEMENT ACQUIS
 5.5 ou 6.0</v>
       </c>
-      <c r="F7" s="160"/>
-      <c r="G7" s="160"/>
-      <c r="H7" s="161" t="str">
+      <c r="F7" s="184"/>
+      <c r="G7" s="184"/>
+      <c r="H7" s="185" t="str">
         <f>[1]INDICATEURS!H7</f>
         <v>SUFFISANT
 4.0, 4.5 ou 5.0</v>
       </c>
-      <c r="I7" s="162"/>
-      <c r="J7" s="162"/>
-      <c r="K7" s="163" t="str">
+      <c r="I7" s="186"/>
+      <c r="J7" s="186"/>
+      <c r="K7" s="187" t="str">
         <f>[1]INDICATEURS!K7</f>
         <v>INSUFFISANT
 2.5, 3.0 ou 3.5</v>
       </c>
-      <c r="L7" s="164"/>
-      <c r="M7" s="164"/>
-      <c r="N7" s="165" t="str">
+      <c r="L7" s="188"/>
+      <c r="M7" s="188"/>
+      <c r="N7" s="189" t="str">
         <f>[1]INDICATEURS!N7</f>
         <v>NON ACQUIS
 1.0, 1.5, ou 2.0</v>
       </c>
-      <c r="O7" s="166"/>
-      <c r="P7" s="166"/>
+      <c r="O7" s="190"/>
+      <c r="P7" s="190"/>
       <c r="Q7" s="52" t="str">
         <f>[1]INDICATEURS!Q7</f>
         <v>Coeff.</v>
@@ -2492,11 +2492,11 @@
     </row>
     <row r="8" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="167" t="str">
+      <c r="B8" s="169" t="str">
         <f>[1]INDICATEURS!B8</f>
         <v>COMPÉTENCES</v>
       </c>
-      <c r="C8" s="170" t="str">
+      <c r="C8" s="172" t="str">
         <f>[1]INDICATEURS!C8</f>
         <v>PROFESSIONNELLES</v>
       </c>
@@ -2521,9 +2521,7 @@
         <f>[1]INDICATEURS!I8</f>
         <v>Respecte les délais fixés avec un rythme normal</v>
       </c>
-      <c r="J8" s="61">
-        <v>4</v>
-      </c>
+      <c r="J8" s="61"/>
       <c r="K8" s="125" t="s">
         <v>15</v>
       </c>
@@ -2531,7 +2529,9 @@
         <f>[1]INDICATEURS!L8</f>
         <v>Travaille lentement et ne respecte pas vraiment les délais</v>
       </c>
-      <c r="M8" s="63"/>
+      <c r="M8" s="63">
+        <v>3.5</v>
+      </c>
       <c r="N8" s="125" t="s">
         <v>15</v>
       </c>
@@ -2546,14 +2546,14 @@
       </c>
       <c r="R8" s="67">
         <f t="shared" ref="R8:R15" si="0">IF(COUNT(G8,J8,M8,P8)=0,"",IF(COUNT(G8,J8,M8,P8)&lt;&gt;1,"ERREUR",Q8*(G8+J8+M8+P8)))</f>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="S8" s="13"/>
     </row>
     <row r="9" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="171"/>
+      <c r="B9" s="170"/>
+      <c r="C9" s="173"/>
       <c r="D9" s="68" t="str">
         <f>[1]INDICATEURS!D9</f>
         <v>Conscience professionnelle
@@ -2606,8 +2606,8 @@
     </row>
     <row r="10" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="168"/>
-      <c r="C10" s="171"/>
+      <c r="B10" s="170"/>
+      <c r="C10" s="173"/>
       <c r="D10" s="68" t="str">
         <f>[1]INDICATEURS!D10</f>
         <v>Connaissances professionnelles
@@ -2660,8 +2660,8 @@
     </row>
     <row r="11" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="168"/>
-      <c r="C11" s="172" t="str">
+      <c r="B11" s="170"/>
+      <c r="C11" s="174" t="str">
         <f>[1]INDICATEURS!C11</f>
         <v>METHODOLOGIQUES</v>
       </c>
@@ -2716,8 +2716,8 @@
     </row>
     <row r="12" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="168"/>
-      <c r="C12" s="173"/>
+      <c r="B12" s="170"/>
+      <c r="C12" s="175"/>
       <c r="D12" s="93" t="str">
         <f>[1]INDICATEURS!D12</f>
         <v>Expression orale et écrite
@@ -2770,8 +2770,8 @@
     </row>
     <row r="13" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A13" s="7"/>
-      <c r="B13" s="168"/>
-      <c r="C13" s="174"/>
+      <c r="B13" s="170"/>
+      <c r="C13" s="176"/>
       <c r="D13" s="105" t="str">
         <f>[1]INDICATEURS!D13</f>
         <v>Approche écologique et économique
@@ -2822,7 +2822,7 @@
     </row>
     <row r="14" spans="1:23" ht="100.15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="7"/>
-      <c r="B14" s="168"/>
+      <c r="B14" s="170"/>
       <c r="C14" s="116" t="str">
         <f>[1]INDICATEURS!C14</f>
         <v>SOCIALES</v>
@@ -2879,7 +2879,7 @@
     </row>
     <row r="15" spans="1:23" ht="120" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="7"/>
-      <c r="B15" s="169"/>
+      <c r="B15" s="171"/>
       <c r="C15" s="116" t="str">
         <f>[1]INDICATEURS!C15</f>
         <v>PERSONNELLES</v>
@@ -2953,7 +2953,7 @@
       <c r="M17" s="136"/>
       <c r="N17" s="138"/>
       <c r="O17" s="139"/>
-      <c r="P17" s="175" t="s">
+      <c r="P17" s="177" t="s">
         <v>10</v>
       </c>
       <c r="Q17" s="140"/>
@@ -2969,45 +2969,45 @@
       <c r="M18" s="137"/>
       <c r="N18" s="137"/>
       <c r="O18" s="137"/>
-      <c r="P18" s="175"/>
+      <c r="P18" s="177"/>
       <c r="Q18" s="140"/>
       <c r="R18" s="140"/>
       <c r="S18" s="13"/>
     </row>
     <row r="19" spans="1:19" ht="30" customHeight="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="176"/>
-      <c r="C19" s="176"/>
-      <c r="D19" s="176"/>
-      <c r="E19" s="176"/>
-      <c r="F19" s="176"/>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176"/>
-      <c r="K19" s="177" t="s">
+      <c r="B19" s="178"/>
+      <c r="C19" s="178"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="178"/>
+      <c r="F19" s="178"/>
+      <c r="G19" s="178"/>
+      <c r="H19" s="178"/>
+      <c r="I19" s="178"/>
+      <c r="K19" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="L19" s="177"/>
-      <c r="M19" s="178">
+      <c r="L19" s="179"/>
+      <c r="M19" s="180">
         <v>44897</v>
       </c>
-      <c r="N19" s="178"/>
-      <c r="O19" s="178"/>
-      <c r="P19" s="175"/>
+      <c r="N19" s="180"/>
+      <c r="O19" s="180"/>
+      <c r="P19" s="177"/>
       <c r="Q19" s="140"/>
       <c r="R19" s="140"/>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="1:19" ht="30" customHeight="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="179"/>
-      <c r="C20" s="179"/>
-      <c r="D20" s="179"/>
-      <c r="E20" s="179"/>
-      <c r="F20" s="179"/>
-      <c r="G20" s="179"/>
-      <c r="H20" s="179"/>
-      <c r="I20" s="179"/>
+      <c r="B20" s="166"/>
+      <c r="C20" s="166"/>
+      <c r="D20" s="166"/>
+      <c r="E20" s="166"/>
+      <c r="F20" s="166"/>
+      <c r="G20" s="166"/>
+      <c r="H20" s="166"/>
+      <c r="I20" s="166"/>
       <c r="K20" s="143"/>
       <c r="L20" s="143"/>
       <c r="M20" s="137"/>
@@ -3020,23 +3020,23 @@
     </row>
     <row r="21" spans="1:19" ht="30" customHeight="1">
       <c r="A21" s="7"/>
-      <c r="B21" s="179"/>
-      <c r="C21" s="179"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="179"/>
-      <c r="F21" s="179"/>
-      <c r="G21" s="179"/>
-      <c r="H21" s="179"/>
-      <c r="I21" s="179"/>
-      <c r="K21" s="180" t="s">
+      <c r="B21" s="166"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="166"/>
+      <c r="E21" s="166"/>
+      <c r="F21" s="166"/>
+      <c r="G21" s="166"/>
+      <c r="H21" s="166"/>
+      <c r="I21" s="166"/>
+      <c r="K21" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="180"/>
-      <c r="M21" s="181" t="s">
+      <c r="L21" s="168"/>
+      <c r="M21" s="167" t="s">
         <v>14</v>
       </c>
-      <c r="N21" s="181"/>
-      <c r="O21" s="181"/>
+      <c r="N21" s="167"/>
+      <c r="O21" s="167"/>
       <c r="P21" s="146"/>
       <c r="Q21" s="147"/>
       <c r="R21" s="147"/>
@@ -3044,14 +3044,14 @@
     </row>
     <row r="22" spans="1:19" ht="30" customHeight="1">
       <c r="A22" s="7"/>
-      <c r="B22" s="179"/>
-      <c r="C22" s="179"/>
-      <c r="D22" s="179"/>
-      <c r="E22" s="179"/>
-      <c r="F22" s="179"/>
-      <c r="G22" s="179"/>
-      <c r="H22" s="179"/>
-      <c r="I22" s="179"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="166"/>
+      <c r="D22" s="166"/>
+      <c r="E22" s="166"/>
+      <c r="F22" s="166"/>
+      <c r="G22" s="166"/>
+      <c r="H22" s="166"/>
+      <c r="I22" s="166"/>
       <c r="K22" s="137"/>
       <c r="L22" s="137"/>
       <c r="M22" s="137"/>
@@ -3063,112 +3063,112 @@
     </row>
     <row r="23" spans="1:19" ht="30" customHeight="1">
       <c r="A23" s="7"/>
-      <c r="B23" s="179"/>
-      <c r="C23" s="179"/>
-      <c r="D23" s="179"/>
-      <c r="E23" s="179"/>
-      <c r="F23" s="179"/>
-      <c r="G23" s="179"/>
-      <c r="H23" s="179"/>
-      <c r="I23" s="179"/>
+      <c r="B23" s="166"/>
+      <c r="C23" s="166"/>
+      <c r="D23" s="166"/>
+      <c r="E23" s="166"/>
+      <c r="F23" s="166"/>
+      <c r="G23" s="166"/>
+      <c r="H23" s="166"/>
+      <c r="I23" s="166"/>
       <c r="J23" s="148"/>
       <c r="K23" s="136" t="s">
         <v>13</v>
       </c>
       <c r="L23" s="149"/>
-      <c r="M23" s="181"/>
-      <c r="N23" s="181"/>
-      <c r="O23" s="181"/>
-      <c r="P23" s="183"/>
-      <c r="Q23" s="185">
+      <c r="M23" s="167"/>
+      <c r="N23" s="167"/>
+      <c r="O23" s="167"/>
+      <c r="P23" s="158"/>
+      <c r="Q23" s="160">
         <f>IF(COUNT(R8:R15)=8,MROUND(SUM(R8:R15)/SUM(Q8:Q15),0.5),"")</f>
         <v>4.5</v>
       </c>
-      <c r="R23" s="186"/>
+      <c r="R23" s="161"/>
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:19" ht="30" customHeight="1">
       <c r="A24" s="7"/>
-      <c r="B24" s="179"/>
-      <c r="C24" s="179"/>
-      <c r="D24" s="179"/>
-      <c r="E24" s="179"/>
-      <c r="F24" s="179"/>
-      <c r="G24" s="179"/>
-      <c r="H24" s="179"/>
-      <c r="I24" s="179"/>
+      <c r="B24" s="166"/>
+      <c r="C24" s="166"/>
+      <c r="D24" s="166"/>
+      <c r="E24" s="166"/>
+      <c r="F24" s="166"/>
+      <c r="G24" s="166"/>
+      <c r="H24" s="166"/>
+      <c r="I24" s="166"/>
       <c r="J24" s="150"/>
       <c r="K24" s="137"/>
       <c r="L24" s="136"/>
       <c r="M24" s="136"/>
       <c r="N24" s="136"/>
       <c r="O24" s="151"/>
-      <c r="P24" s="184"/>
-      <c r="Q24" s="187"/>
-      <c r="R24" s="188"/>
+      <c r="P24" s="159"/>
+      <c r="Q24" s="162"/>
+      <c r="R24" s="163"/>
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="1:19" ht="28.5" customHeight="1">
       <c r="A25" s="7"/>
-      <c r="B25" s="179"/>
-      <c r="C25" s="179"/>
-      <c r="D25" s="179"/>
-      <c r="E25" s="179"/>
-      <c r="F25" s="179"/>
-      <c r="G25" s="179"/>
-      <c r="H25" s="179"/>
-      <c r="I25" s="179"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="166"/>
+      <c r="D25" s="166"/>
+      <c r="E25" s="166"/>
+      <c r="F25" s="166"/>
+      <c r="G25" s="166"/>
+      <c r="H25" s="166"/>
+      <c r="I25" s="166"/>
       <c r="J25" s="148"/>
       <c r="K25" s="137"/>
       <c r="L25" s="149"/>
       <c r="M25" s="137"/>
       <c r="N25" s="152"/>
       <c r="O25" s="151"/>
-      <c r="P25" s="184"/>
-      <c r="Q25" s="187"/>
-      <c r="R25" s="188"/>
+      <c r="P25" s="159"/>
+      <c r="Q25" s="162"/>
+      <c r="R25" s="163"/>
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="1:19" ht="30" customHeight="1">
       <c r="A26" s="7"/>
-      <c r="B26" s="179"/>
-      <c r="C26" s="179"/>
-      <c r="D26" s="179"/>
-      <c r="E26" s="179"/>
-      <c r="F26" s="179"/>
-      <c r="G26" s="179"/>
-      <c r="H26" s="179"/>
-      <c r="I26" s="179"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="166"/>
+      <c r="D26" s="166"/>
+      <c r="E26" s="166"/>
+      <c r="F26" s="166"/>
+      <c r="G26" s="166"/>
+      <c r="H26" s="166"/>
+      <c r="I26" s="166"/>
       <c r="J26" s="150"/>
       <c r="K26" s="153"/>
       <c r="L26" s="137"/>
       <c r="M26" s="137"/>
       <c r="N26" s="152"/>
       <c r="O26" s="151"/>
-      <c r="P26" s="184"/>
-      <c r="Q26" s="187"/>
-      <c r="R26" s="188"/>
+      <c r="P26" s="159"/>
+      <c r="Q26" s="162"/>
+      <c r="R26" s="163"/>
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="1:19" ht="30" customHeight="1">
       <c r="A27" s="7"/>
-      <c r="B27" s="179"/>
-      <c r="C27" s="179"/>
-      <c r="D27" s="179"/>
-      <c r="E27" s="179"/>
-      <c r="F27" s="179"/>
-      <c r="G27" s="179"/>
-      <c r="H27" s="179"/>
-      <c r="I27" s="179"/>
+      <c r="B27" s="166"/>
+      <c r="C27" s="166"/>
+      <c r="D27" s="166"/>
+      <c r="E27" s="166"/>
+      <c r="F27" s="166"/>
+      <c r="G27" s="166"/>
+      <c r="H27" s="166"/>
+      <c r="I27" s="166"/>
       <c r="J27" s="150"/>
       <c r="K27" s="153"/>
       <c r="L27" s="137"/>
       <c r="M27" s="137"/>
       <c r="N27" s="152"/>
       <c r="O27" s="151"/>
-      <c r="P27" s="184"/>
-      <c r="Q27" s="189"/>
-      <c r="R27" s="190"/>
+      <c r="P27" s="159"/>
+      <c r="Q27" s="164"/>
+      <c r="R27" s="165"/>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:19" ht="9.75" hidden="1" customHeight="1" thickBot="1">
@@ -3228,14 +3228,14 @@
     <row r="42" spans="1:19" ht="12.75"/>
     <row r="43" spans="1:19" ht="12.75"/>
     <row r="44" spans="1:19" ht="12.75">
-      <c r="L44" s="182"/>
-      <c r="M44" s="182"/>
-      <c r="N44" s="182"/>
+      <c r="L44" s="157"/>
+      <c r="M44" s="157"/>
+      <c r="N44" s="157"/>
     </row>
     <row r="45" spans="1:19" ht="12.75">
-      <c r="L45" s="182"/>
-      <c r="M45" s="182"/>
-      <c r="N45" s="182"/>
+      <c r="L45" s="157"/>
+      <c r="M45" s="157"/>
+      <c r="N45" s="157"/>
     </row>
     <row r="46" spans="1:19" ht="12.75"/>
     <row r="47" spans="1:19" ht="12.75"/>
@@ -3278,6 +3278,24 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="27">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="P17:P19"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="B22:I22"/>
     <mergeCell ref="L44:N45"/>
     <mergeCell ref="P23:P27"/>
     <mergeCell ref="Q23:R27"/>
@@ -3287,24 +3305,6 @@
     <mergeCell ref="B27:I27"/>
     <mergeCell ref="B23:I23"/>
     <mergeCell ref="M23:O23"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="P17:P19"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <conditionalFormatting sqref="Q23:R27">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -3351,6 +3351,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E529CC47EA4E614CBF50FAFAB9B8F32B" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f813ab756c42af8af494d6605e22e37b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98d92101-24da-4498-9971-a24673344bd8" xmlns:ns3="dfa80de1-e9bb-4cf2-893d-d06220b3971a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="808c042e6474ee35eb4b0b0b71aaa865" ns2:_="" ns3:_="">
     <xsd:import namespace="98d92101-24da-4498-9971-a24673344bd8"/>
@@ -3527,15 +3536,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB127613-3E42-413C-AA19-20FDD7FDB721}">
   <ds:schemaRefs>
@@ -3548,6 +3548,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D42627D-2FD8-4CD0-813D-983EAA15F567}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E97D3F8-EB60-4F3F-861E-88C92BD29808}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3564,12 +3572,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D42627D-2FD8-4CD0-813D-983EAA15F567}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>